<commit_message>
change on finance and address to track iuran per month
</commit_message>
<xml_diff>
--- a/server/public/templates/Finance_template.xlsx
+++ b/server/public/templates/Finance_template.xlsx
@@ -16,6 +16,24 @@
     <author/>
   </authors>
   <commentList>
+    <comment authorId="0" ref="G1">
+      <text>
+        <t xml:space="preserve">Isi jika Jenis pendapatan adalah Iuran. isi sesuai alamat di menu Alamat
+	-Ikhsan Muhammad</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="F1">
+      <text>
+        <t xml:space="preserve">Di isi jika Jenis Pendapatan adalah Iuran. isi dengan MM-YYYY (05-2025)
+	-Ikhsan Muhammad</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="E1">
+      <text>
+        <t xml:space="preserve">Di isi jika kategori yang dipilih adalah Pendapatan
+	-Ikhsan Muhammad</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="C1">
       <text>
         <t xml:space="preserve">Isikan angka saja tanpa titik / koma (1000000)
@@ -33,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Tanggal</t>
   </si>
@@ -47,7 +65,13 @@
     <t>Keterangan</t>
   </si>
   <si>
-    <t>NIK</t>
+    <t>Jenis Pendapatan</t>
+  </si>
+  <si>
+    <t>Bulan</t>
+  </si>
+  <si>
+    <t>Alamat</t>
   </si>
 </sst>
 </file>
@@ -129,7 +153,18 @@
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -361,6 +396,12 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="3"/>
@@ -368,6 +409,8 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
     </row>
     <row r="3">
       <c r="A3" s="3"/>
@@ -375,6 +418,8 @@
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
     </row>
     <row r="4">
       <c r="A4" s="3"/>
@@ -382,6 +427,8 @@
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5">
       <c r="A5" s="3"/>
@@ -389,6 +436,8 @@
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
     </row>
     <row r="6">
       <c r="A6" s="3"/>
@@ -396,6 +445,8 @@
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
     </row>
     <row r="7">
       <c r="A7" s="3"/>
@@ -403,6 +454,8 @@
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
     </row>
     <row r="8">
       <c r="A8" s="3"/>
@@ -410,6 +463,8 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
     </row>
     <row r="9">
       <c r="A9" s="3"/>
@@ -417,6 +472,8 @@
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
     </row>
     <row r="10">
       <c r="A10" s="3"/>
@@ -424,6 +481,8 @@
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
     </row>
     <row r="11">
       <c r="A11" s="3"/>
@@ -431,6 +490,8 @@
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
     </row>
     <row r="12">
       <c r="A12" s="3"/>
@@ -438,6 +499,8 @@
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
     </row>
     <row r="13">
       <c r="A13" s="3"/>
@@ -445,6 +508,8 @@
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
     </row>
     <row r="14">
       <c r="A14" s="3"/>
@@ -452,6 +517,8 @@
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
     </row>
     <row r="15">
       <c r="A15" s="3"/>
@@ -459,6 +526,8 @@
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
     </row>
     <row r="16">
       <c r="A16" s="3"/>
@@ -466,6 +535,8 @@
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
     </row>
     <row r="17">
       <c r="A17" s="3"/>
@@ -473,6 +544,8 @@
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
     </row>
     <row r="18">
       <c r="A18" s="3"/>
@@ -480,6 +553,8 @@
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
     </row>
     <row r="19">
       <c r="A19" s="3"/>
@@ -487,6 +562,8 @@
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
     </row>
     <row r="20">
       <c r="A20" s="3"/>
@@ -494,6 +571,8 @@
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
     </row>
     <row r="21">
       <c r="A21" s="3"/>
@@ -501,6 +580,8 @@
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
     </row>
     <row r="22">
       <c r="A22" s="3"/>
@@ -508,6 +589,8 @@
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
     </row>
     <row r="23">
       <c r="A23" s="3"/>
@@ -515,6 +598,8 @@
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
     </row>
     <row r="24">
       <c r="A24" s="3"/>
@@ -522,6 +607,8 @@
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
     </row>
     <row r="25">
       <c r="A25" s="3"/>
@@ -529,6 +616,8 @@
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
     </row>
     <row r="26">
       <c r="A26" s="3"/>
@@ -536,6 +625,8 @@
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
     </row>
     <row r="27">
       <c r="A27" s="3"/>
@@ -543,6 +634,8 @@
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
     </row>
     <row r="28">
       <c r="A28" s="3"/>
@@ -550,6 +643,8 @@
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
     </row>
     <row r="29">
       <c r="A29" s="3"/>
@@ -557,6 +652,8 @@
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
     </row>
     <row r="30">
       <c r="A30" s="3"/>
@@ -564,6 +661,8 @@
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
     </row>
     <row r="31">
       <c r="A31" s="3"/>
@@ -571,6 +670,8 @@
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
     </row>
     <row r="32">
       <c r="A32" s="3"/>
@@ -578,6 +679,8 @@
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
     </row>
     <row r="33">
       <c r="A33" s="3"/>
@@ -585,6 +688,8 @@
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
     </row>
     <row r="34">
       <c r="A34" s="3"/>
@@ -592,6 +697,8 @@
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
     </row>
     <row r="35">
       <c r="A35" s="3"/>
@@ -599,6 +706,8 @@
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
     </row>
     <row r="36">
       <c r="A36" s="3"/>
@@ -606,6 +715,8 @@
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
     </row>
     <row r="37">
       <c r="A37" s="3"/>
@@ -613,6 +724,8 @@
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
     </row>
     <row r="38">
       <c r="A38" s="3"/>
@@ -620,6 +733,8 @@
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
     </row>
     <row r="39">
       <c r="A39" s="3"/>
@@ -627,6 +742,8 @@
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
     </row>
     <row r="40">
       <c r="A40" s="3"/>
@@ -634,6 +751,8 @@
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
     </row>
     <row r="41">
       <c r="A41" s="3"/>
@@ -641,6 +760,8 @@
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
     </row>
     <row r="42">
       <c r="A42" s="3"/>
@@ -648,6 +769,8 @@
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
     </row>
     <row r="43">
       <c r="A43" s="3"/>
@@ -655,6 +778,8 @@
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
     </row>
     <row r="44">
       <c r="A44" s="3"/>
@@ -662,6 +787,8 @@
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
     </row>
     <row r="45">
       <c r="A45" s="3"/>
@@ -669,6 +796,8 @@
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
     </row>
     <row r="46">
       <c r="A46" s="3"/>
@@ -676,6 +805,8 @@
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
     </row>
     <row r="47">
       <c r="A47" s="3"/>
@@ -683,6 +814,8 @@
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
     </row>
     <row r="48">
       <c r="A48" s="3"/>
@@ -690,6 +823,8 @@
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
     </row>
     <row r="49">
       <c r="A49" s="3"/>
@@ -697,6 +832,8 @@
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
     </row>
     <row r="50">
       <c r="A50" s="3"/>
@@ -704,6 +841,8 @@
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
     </row>
     <row r="51">
       <c r="A51" s="3"/>
@@ -711,6 +850,8 @@
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
     </row>
     <row r="52">
       <c r="A52" s="3"/>
@@ -718,6 +859,8 @@
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
     </row>
     <row r="53">
       <c r="A53" s="3"/>
@@ -725,6 +868,8 @@
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
     </row>
     <row r="54">
       <c r="A54" s="3"/>
@@ -732,6 +877,8 @@
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
     </row>
     <row r="55">
       <c r="A55" s="3"/>
@@ -739,6 +886,8 @@
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
     </row>
     <row r="56">
       <c r="A56" s="3"/>
@@ -746,6 +895,8 @@
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
     </row>
     <row r="57">
       <c r="A57" s="3"/>
@@ -753,6 +904,8 @@
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
     </row>
     <row r="58">
       <c r="A58" s="3"/>
@@ -760,6 +913,8 @@
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
     </row>
     <row r="59">
       <c r="A59" s="3"/>
@@ -767,6 +922,8 @@
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
     </row>
     <row r="60">
       <c r="A60" s="3"/>
@@ -774,6 +931,8 @@
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
     </row>
     <row r="61">
       <c r="A61" s="3"/>
@@ -781,6 +940,8 @@
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
     </row>
     <row r="62">
       <c r="A62" s="3"/>
@@ -788,6 +949,8 @@
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
+      <c r="F62" s="3"/>
+      <c r="G62" s="3"/>
     </row>
     <row r="63">
       <c r="A63" s="3"/>
@@ -795,6 +958,8 @@
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
     </row>
     <row r="64">
       <c r="A64" s="3"/>
@@ -802,6 +967,8 @@
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
     </row>
     <row r="65">
       <c r="A65" s="3"/>
@@ -809,6 +976,8 @@
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
+      <c r="F65" s="3"/>
+      <c r="G65" s="3"/>
     </row>
     <row r="66">
       <c r="A66" s="3"/>
@@ -816,6 +985,8 @@
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3"/>
     </row>
     <row r="67">
       <c r="A67" s="3"/>
@@ -823,6 +994,8 @@
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3"/>
     </row>
     <row r="68">
       <c r="A68" s="3"/>
@@ -830,6 +1003,8 @@
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
+      <c r="G68" s="3"/>
     </row>
     <row r="69">
       <c r="A69" s="3"/>
@@ -837,6 +1012,8 @@
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+      <c r="G69" s="3"/>
     </row>
     <row r="70">
       <c r="A70" s="3"/>
@@ -844,6 +1021,8 @@
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3"/>
     </row>
     <row r="71">
       <c r="A71" s="3"/>
@@ -851,6 +1030,8 @@
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
       <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
+      <c r="G71" s="3"/>
     </row>
     <row r="72">
       <c r="A72" s="3"/>
@@ -858,6 +1039,8 @@
       <c r="C72" s="3"/>
       <c r="D72" s="3"/>
       <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+      <c r="G72" s="3"/>
     </row>
     <row r="73">
       <c r="A73" s="3"/>
@@ -865,6 +1048,8 @@
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="3"/>
     </row>
     <row r="74">
       <c r="A74" s="3"/>
@@ -872,6 +1057,8 @@
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
       <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
     </row>
     <row r="75">
       <c r="A75" s="3"/>
@@ -879,6 +1066,8 @@
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
       <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3"/>
     </row>
     <row r="76">
       <c r="A76" s="3"/>
@@ -886,6 +1075,8 @@
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
       <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+      <c r="G76" s="3"/>
     </row>
     <row r="77">
       <c r="A77" s="3"/>
@@ -893,6 +1084,8 @@
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
+      <c r="F77" s="3"/>
+      <c r="G77" s="3"/>
     </row>
     <row r="78">
       <c r="A78" s="3"/>
@@ -900,6 +1093,8 @@
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
       <c r="E78" s="3"/>
+      <c r="F78" s="3"/>
+      <c r="G78" s="3"/>
     </row>
     <row r="79">
       <c r="A79" s="3"/>
@@ -907,6 +1102,8 @@
       <c r="C79" s="3"/>
       <c r="D79" s="3"/>
       <c r="E79" s="3"/>
+      <c r="F79" s="3"/>
+      <c r="G79" s="3"/>
     </row>
     <row r="80">
       <c r="A80" s="3"/>
@@ -914,6 +1111,8 @@
       <c r="C80" s="3"/>
       <c r="D80" s="3"/>
       <c r="E80" s="3"/>
+      <c r="F80" s="3"/>
+      <c r="G80" s="3"/>
     </row>
     <row r="81">
       <c r="A81" s="3"/>
@@ -921,6 +1120,8 @@
       <c r="C81" s="3"/>
       <c r="D81" s="3"/>
       <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
+      <c r="G81" s="3"/>
     </row>
     <row r="82">
       <c r="A82" s="3"/>
@@ -928,6 +1129,8 @@
       <c r="C82" s="3"/>
       <c r="D82" s="3"/>
       <c r="E82" s="3"/>
+      <c r="F82" s="3"/>
+      <c r="G82" s="3"/>
     </row>
     <row r="83">
       <c r="A83" s="3"/>
@@ -935,6 +1138,8 @@
       <c r="C83" s="3"/>
       <c r="D83" s="3"/>
       <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
+      <c r="G83" s="3"/>
     </row>
     <row r="84">
       <c r="A84" s="3"/>
@@ -942,6 +1147,8 @@
       <c r="C84" s="3"/>
       <c r="D84" s="3"/>
       <c r="E84" s="3"/>
+      <c r="F84" s="3"/>
+      <c r="G84" s="3"/>
     </row>
     <row r="85">
       <c r="A85" s="3"/>
@@ -949,6 +1156,8 @@
       <c r="C85" s="3"/>
       <c r="D85" s="3"/>
       <c r="E85" s="3"/>
+      <c r="F85" s="3"/>
+      <c r="G85" s="3"/>
     </row>
     <row r="86">
       <c r="A86" s="3"/>
@@ -956,6 +1165,8 @@
       <c r="C86" s="3"/>
       <c r="D86" s="3"/>
       <c r="E86" s="3"/>
+      <c r="F86" s="3"/>
+      <c r="G86" s="3"/>
     </row>
     <row r="87">
       <c r="A87" s="3"/>
@@ -963,6 +1174,8 @@
       <c r="C87" s="3"/>
       <c r="D87" s="3"/>
       <c r="E87" s="3"/>
+      <c r="F87" s="3"/>
+      <c r="G87" s="3"/>
     </row>
     <row r="88">
       <c r="A88" s="3"/>
@@ -970,6 +1183,8 @@
       <c r="C88" s="3"/>
       <c r="D88" s="3"/>
       <c r="E88" s="3"/>
+      <c r="F88" s="3"/>
+      <c r="G88" s="3"/>
     </row>
     <row r="89">
       <c r="A89" s="3"/>
@@ -977,6 +1192,8 @@
       <c r="C89" s="3"/>
       <c r="D89" s="3"/>
       <c r="E89" s="3"/>
+      <c r="F89" s="3"/>
+      <c r="G89" s="3"/>
     </row>
     <row r="90">
       <c r="A90" s="3"/>
@@ -984,6 +1201,8 @@
       <c r="C90" s="3"/>
       <c r="D90" s="3"/>
       <c r="E90" s="3"/>
+      <c r="F90" s="3"/>
+      <c r="G90" s="3"/>
     </row>
     <row r="91">
       <c r="A91" s="3"/>
@@ -991,6 +1210,8 @@
       <c r="C91" s="3"/>
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
+      <c r="F91" s="3"/>
+      <c r="G91" s="3"/>
     </row>
     <row r="92">
       <c r="A92" s="3"/>
@@ -998,6 +1219,8 @@
       <c r="C92" s="3"/>
       <c r="D92" s="3"/>
       <c r="E92" s="3"/>
+      <c r="F92" s="3"/>
+      <c r="G92" s="3"/>
     </row>
     <row r="93">
       <c r="A93" s="3"/>
@@ -1005,6 +1228,8 @@
       <c r="C93" s="3"/>
       <c r="D93" s="3"/>
       <c r="E93" s="3"/>
+      <c r="F93" s="3"/>
+      <c r="G93" s="3"/>
     </row>
     <row r="94">
       <c r="A94" s="3"/>
@@ -1012,6 +1237,8 @@
       <c r="C94" s="3"/>
       <c r="D94" s="3"/>
       <c r="E94" s="3"/>
+      <c r="F94" s="3"/>
+      <c r="G94" s="3"/>
     </row>
     <row r="95">
       <c r="A95" s="3"/>
@@ -1019,6 +1246,8 @@
       <c r="C95" s="3"/>
       <c r="D95" s="3"/>
       <c r="E95" s="3"/>
+      <c r="F95" s="3"/>
+      <c r="G95" s="3"/>
     </row>
     <row r="96">
       <c r="A96" s="3"/>
@@ -1026,6 +1255,8 @@
       <c r="C96" s="3"/>
       <c r="D96" s="3"/>
       <c r="E96" s="3"/>
+      <c r="F96" s="3"/>
+      <c r="G96" s="3"/>
     </row>
     <row r="97">
       <c r="A97" s="3"/>
@@ -1033,6 +1264,8 @@
       <c r="C97" s="3"/>
       <c r="D97" s="3"/>
       <c r="E97" s="3"/>
+      <c r="F97" s="3"/>
+      <c r="G97" s="3"/>
     </row>
     <row r="98">
       <c r="A98" s="3"/>
@@ -1040,6 +1273,8 @@
       <c r="C98" s="3"/>
       <c r="D98" s="3"/>
       <c r="E98" s="3"/>
+      <c r="F98" s="3"/>
+      <c r="G98" s="3"/>
     </row>
     <row r="99">
       <c r="A99" s="3"/>
@@ -1047,6 +1282,8 @@
       <c r="C99" s="3"/>
       <c r="D99" s="3"/>
       <c r="E99" s="3"/>
+      <c r="F99" s="3"/>
+      <c r="G99" s="3"/>
     </row>
     <row r="100">
       <c r="A100" s="3"/>
@@ -1054,6 +1291,8 @@
       <c r="C100" s="3"/>
       <c r="D100" s="3"/>
       <c r="E100" s="3"/>
+      <c r="F100" s="3"/>
+      <c r="G100" s="3"/>
     </row>
     <row r="101">
       <c r="A101" s="3"/>
@@ -1061,6 +1300,8 @@
       <c r="C101" s="3"/>
       <c r="D101" s="3"/>
       <c r="E101" s="3"/>
+      <c r="F101" s="3"/>
+      <c r="G101" s="3"/>
     </row>
     <row r="102">
       <c r="A102" s="3"/>
@@ -1068,6 +1309,8 @@
       <c r="C102" s="3"/>
       <c r="D102" s="3"/>
       <c r="E102" s="3"/>
+      <c r="F102" s="3"/>
+      <c r="G102" s="3"/>
     </row>
     <row r="103">
       <c r="A103" s="3"/>
@@ -1075,6 +1318,8 @@
       <c r="C103" s="3"/>
       <c r="D103" s="3"/>
       <c r="E103" s="3"/>
+      <c r="F103" s="3"/>
+      <c r="G103" s="3"/>
     </row>
     <row r="104">
       <c r="A104" s="3"/>
@@ -1082,6 +1327,8 @@
       <c r="C104" s="3"/>
       <c r="D104" s="3"/>
       <c r="E104" s="3"/>
+      <c r="F104" s="3"/>
+      <c r="G104" s="3"/>
     </row>
     <row r="105">
       <c r="A105" s="3"/>
@@ -1089,6 +1336,8 @@
       <c r="C105" s="3"/>
       <c r="D105" s="3"/>
       <c r="E105" s="3"/>
+      <c r="F105" s="3"/>
+      <c r="G105" s="3"/>
     </row>
     <row r="106">
       <c r="A106" s="3"/>
@@ -1096,6 +1345,8 @@
       <c r="C106" s="3"/>
       <c r="D106" s="3"/>
       <c r="E106" s="3"/>
+      <c r="F106" s="3"/>
+      <c r="G106" s="3"/>
     </row>
     <row r="107">
       <c r="A107" s="3"/>
@@ -1103,6 +1354,8 @@
       <c r="C107" s="3"/>
       <c r="D107" s="3"/>
       <c r="E107" s="3"/>
+      <c r="F107" s="3"/>
+      <c r="G107" s="3"/>
     </row>
     <row r="108">
       <c r="A108" s="3"/>
@@ -1110,6 +1363,8 @@
       <c r="C108" s="3"/>
       <c r="D108" s="3"/>
       <c r="E108" s="3"/>
+      <c r="F108" s="3"/>
+      <c r="G108" s="3"/>
     </row>
     <row r="109">
       <c r="A109" s="3"/>
@@ -1117,6 +1372,8 @@
       <c r="C109" s="3"/>
       <c r="D109" s="3"/>
       <c r="E109" s="3"/>
+      <c r="F109" s="3"/>
+      <c r="G109" s="3"/>
     </row>
     <row r="110">
       <c r="A110" s="3"/>
@@ -1124,6 +1381,8 @@
       <c r="C110" s="3"/>
       <c r="D110" s="3"/>
       <c r="E110" s="3"/>
+      <c r="F110" s="3"/>
+      <c r="G110" s="3"/>
     </row>
     <row r="111">
       <c r="A111" s="3"/>
@@ -1131,6 +1390,8 @@
       <c r="C111" s="3"/>
       <c r="D111" s="3"/>
       <c r="E111" s="3"/>
+      <c r="F111" s="3"/>
+      <c r="G111" s="3"/>
     </row>
     <row r="112">
       <c r="A112" s="3"/>
@@ -1138,6 +1399,8 @@
       <c r="C112" s="3"/>
       <c r="D112" s="3"/>
       <c r="E112" s="3"/>
+      <c r="F112" s="3"/>
+      <c r="G112" s="3"/>
     </row>
     <row r="113">
       <c r="A113" s="3"/>
@@ -1145,6 +1408,8 @@
       <c r="C113" s="3"/>
       <c r="D113" s="3"/>
       <c r="E113" s="3"/>
+      <c r="F113" s="3"/>
+      <c r="G113" s="3"/>
     </row>
     <row r="114">
       <c r="A114" s="3"/>
@@ -1152,6 +1417,8 @@
       <c r="C114" s="3"/>
       <c r="D114" s="3"/>
       <c r="E114" s="3"/>
+      <c r="F114" s="3"/>
+      <c r="G114" s="3"/>
     </row>
     <row r="115">
       <c r="A115" s="3"/>
@@ -1159,6 +1426,8 @@
       <c r="C115" s="3"/>
       <c r="D115" s="3"/>
       <c r="E115" s="3"/>
+      <c r="F115" s="3"/>
+      <c r="G115" s="3"/>
     </row>
     <row r="116">
       <c r="A116" s="3"/>
@@ -1166,6 +1435,8 @@
       <c r="C116" s="3"/>
       <c r="D116" s="3"/>
       <c r="E116" s="3"/>
+      <c r="F116" s="3"/>
+      <c r="G116" s="3"/>
     </row>
     <row r="117">
       <c r="A117" s="3"/>
@@ -1173,6 +1444,8 @@
       <c r="C117" s="3"/>
       <c r="D117" s="3"/>
       <c r="E117" s="3"/>
+      <c r="F117" s="3"/>
+      <c r="G117" s="3"/>
     </row>
     <row r="118">
       <c r="A118" s="3"/>
@@ -1180,6 +1453,8 @@
       <c r="C118" s="3"/>
       <c r="D118" s="3"/>
       <c r="E118" s="3"/>
+      <c r="F118" s="3"/>
+      <c r="G118" s="3"/>
     </row>
     <row r="119">
       <c r="A119" s="3"/>
@@ -1187,6 +1462,8 @@
       <c r="C119" s="3"/>
       <c r="D119" s="3"/>
       <c r="E119" s="3"/>
+      <c r="F119" s="3"/>
+      <c r="G119" s="3"/>
     </row>
     <row r="120">
       <c r="A120" s="3"/>
@@ -1194,6 +1471,8 @@
       <c r="C120" s="3"/>
       <c r="D120" s="3"/>
       <c r="E120" s="3"/>
+      <c r="F120" s="3"/>
+      <c r="G120" s="3"/>
     </row>
     <row r="121">
       <c r="A121" s="3"/>
@@ -1201,6 +1480,8 @@
       <c r="C121" s="3"/>
       <c r="D121" s="3"/>
       <c r="E121" s="3"/>
+      <c r="F121" s="3"/>
+      <c r="G121" s="3"/>
     </row>
     <row r="122">
       <c r="A122" s="3"/>
@@ -1208,6 +1489,8 @@
       <c r="C122" s="3"/>
       <c r="D122" s="3"/>
       <c r="E122" s="3"/>
+      <c r="F122" s="3"/>
+      <c r="G122" s="3"/>
     </row>
     <row r="123">
       <c r="A123" s="3"/>
@@ -1215,6 +1498,8 @@
       <c r="C123" s="3"/>
       <c r="D123" s="3"/>
       <c r="E123" s="3"/>
+      <c r="F123" s="3"/>
+      <c r="G123" s="3"/>
     </row>
     <row r="124">
       <c r="A124" s="3"/>
@@ -1222,6 +1507,8 @@
       <c r="C124" s="3"/>
       <c r="D124" s="3"/>
       <c r="E124" s="3"/>
+      <c r="F124" s="3"/>
+      <c r="G124" s="3"/>
     </row>
     <row r="125">
       <c r="A125" s="3"/>
@@ -1229,6 +1516,8 @@
       <c r="C125" s="3"/>
       <c r="D125" s="3"/>
       <c r="E125" s="3"/>
+      <c r="F125" s="3"/>
+      <c r="G125" s="3"/>
     </row>
     <row r="126">
       <c r="A126" s="3"/>
@@ -1236,6 +1525,8 @@
       <c r="C126" s="3"/>
       <c r="D126" s="3"/>
       <c r="E126" s="3"/>
+      <c r="F126" s="3"/>
+      <c r="G126" s="3"/>
     </row>
     <row r="127">
       <c r="A127" s="3"/>
@@ -1243,6 +1534,8 @@
       <c r="C127" s="3"/>
       <c r="D127" s="3"/>
       <c r="E127" s="3"/>
+      <c r="F127" s="3"/>
+      <c r="G127" s="3"/>
     </row>
     <row r="128">
       <c r="A128" s="3"/>
@@ -1250,6 +1543,8 @@
       <c r="C128" s="3"/>
       <c r="D128" s="3"/>
       <c r="E128" s="3"/>
+      <c r="F128" s="3"/>
+      <c r="G128" s="3"/>
     </row>
     <row r="129">
       <c r="A129" s="3"/>
@@ -1257,6 +1552,8 @@
       <c r="C129" s="3"/>
       <c r="D129" s="3"/>
       <c r="E129" s="3"/>
+      <c r="F129" s="3"/>
+      <c r="G129" s="3"/>
     </row>
     <row r="130">
       <c r="A130" s="3"/>
@@ -1264,6 +1561,8 @@
       <c r="C130" s="3"/>
       <c r="D130" s="3"/>
       <c r="E130" s="3"/>
+      <c r="F130" s="3"/>
+      <c r="G130" s="3"/>
     </row>
     <row r="131">
       <c r="A131" s="3"/>
@@ -1271,6 +1570,8 @@
       <c r="C131" s="3"/>
       <c r="D131" s="3"/>
       <c r="E131" s="3"/>
+      <c r="F131" s="3"/>
+      <c r="G131" s="3"/>
     </row>
     <row r="132">
       <c r="A132" s="3"/>
@@ -1278,6 +1579,8 @@
       <c r="C132" s="3"/>
       <c r="D132" s="3"/>
       <c r="E132" s="3"/>
+      <c r="F132" s="3"/>
+      <c r="G132" s="3"/>
     </row>
     <row r="133">
       <c r="A133" s="3"/>
@@ -1285,6 +1588,8 @@
       <c r="C133" s="3"/>
       <c r="D133" s="3"/>
       <c r="E133" s="3"/>
+      <c r="F133" s="3"/>
+      <c r="G133" s="3"/>
     </row>
     <row r="134">
       <c r="A134" s="3"/>
@@ -1292,6 +1597,8 @@
       <c r="C134" s="3"/>
       <c r="D134" s="3"/>
       <c r="E134" s="3"/>
+      <c r="F134" s="3"/>
+      <c r="G134" s="3"/>
     </row>
     <row r="135">
       <c r="A135" s="3"/>
@@ -1299,6 +1606,8 @@
       <c r="C135" s="3"/>
       <c r="D135" s="3"/>
       <c r="E135" s="3"/>
+      <c r="F135" s="3"/>
+      <c r="G135" s="3"/>
     </row>
     <row r="136">
       <c r="A136" s="3"/>
@@ -1306,6 +1615,8 @@
       <c r="C136" s="3"/>
       <c r="D136" s="3"/>
       <c r="E136" s="3"/>
+      <c r="F136" s="3"/>
+      <c r="G136" s="3"/>
     </row>
     <row r="137">
       <c r="A137" s="3"/>
@@ -1313,6 +1624,8 @@
       <c r="C137" s="3"/>
       <c r="D137" s="3"/>
       <c r="E137" s="3"/>
+      <c r="F137" s="3"/>
+      <c r="G137" s="3"/>
     </row>
     <row r="138">
       <c r="A138" s="3"/>
@@ -1320,6 +1633,8 @@
       <c r="C138" s="3"/>
       <c r="D138" s="3"/>
       <c r="E138" s="3"/>
+      <c r="F138" s="3"/>
+      <c r="G138" s="3"/>
     </row>
     <row r="139">
       <c r="A139" s="3"/>
@@ -1327,6 +1642,8 @@
       <c r="C139" s="3"/>
       <c r="D139" s="3"/>
       <c r="E139" s="3"/>
+      <c r="F139" s="3"/>
+      <c r="G139" s="3"/>
     </row>
     <row r="140">
       <c r="A140" s="3"/>
@@ -1334,6 +1651,8 @@
       <c r="C140" s="3"/>
       <c r="D140" s="3"/>
       <c r="E140" s="3"/>
+      <c r="F140" s="3"/>
+      <c r="G140" s="3"/>
     </row>
     <row r="141">
       <c r="A141" s="3"/>
@@ -1341,6 +1660,8 @@
       <c r="C141" s="3"/>
       <c r="D141" s="3"/>
       <c r="E141" s="3"/>
+      <c r="F141" s="3"/>
+      <c r="G141" s="3"/>
     </row>
     <row r="142">
       <c r="A142" s="3"/>
@@ -1348,6 +1669,8 @@
       <c r="C142" s="3"/>
       <c r="D142" s="3"/>
       <c r="E142" s="3"/>
+      <c r="F142" s="3"/>
+      <c r="G142" s="3"/>
     </row>
     <row r="143">
       <c r="A143" s="3"/>
@@ -1355,6 +1678,8 @@
       <c r="C143" s="3"/>
       <c r="D143" s="3"/>
       <c r="E143" s="3"/>
+      <c r="F143" s="3"/>
+      <c r="G143" s="3"/>
     </row>
     <row r="144">
       <c r="A144" s="3"/>
@@ -1362,6 +1687,8 @@
       <c r="C144" s="3"/>
       <c r="D144" s="3"/>
       <c r="E144" s="3"/>
+      <c r="F144" s="3"/>
+      <c r="G144" s="3"/>
     </row>
     <row r="145">
       <c r="A145" s="3"/>
@@ -1369,6 +1696,8 @@
       <c r="C145" s="3"/>
       <c r="D145" s="3"/>
       <c r="E145" s="3"/>
+      <c r="F145" s="3"/>
+      <c r="G145" s="3"/>
     </row>
     <row r="146">
       <c r="A146" s="3"/>
@@ -1376,6 +1705,8 @@
       <c r="C146" s="3"/>
       <c r="D146" s="3"/>
       <c r="E146" s="3"/>
+      <c r="F146" s="3"/>
+      <c r="G146" s="3"/>
     </row>
     <row r="147">
       <c r="A147" s="3"/>
@@ -1383,6 +1714,8 @@
       <c r="C147" s="3"/>
       <c r="D147" s="3"/>
       <c r="E147" s="3"/>
+      <c r="F147" s="3"/>
+      <c r="G147" s="3"/>
     </row>
     <row r="148">
       <c r="A148" s="3"/>
@@ -1390,6 +1723,8 @@
       <c r="C148" s="3"/>
       <c r="D148" s="3"/>
       <c r="E148" s="3"/>
+      <c r="F148" s="3"/>
+      <c r="G148" s="3"/>
     </row>
     <row r="149">
       <c r="A149" s="3"/>
@@ -1397,6 +1732,8 @@
       <c r="C149" s="3"/>
       <c r="D149" s="3"/>
       <c r="E149" s="3"/>
+      <c r="F149" s="3"/>
+      <c r="G149" s="3"/>
     </row>
     <row r="150">
       <c r="A150" s="3"/>
@@ -1404,6 +1741,8 @@
       <c r="C150" s="3"/>
       <c r="D150" s="3"/>
       <c r="E150" s="3"/>
+      <c r="F150" s="3"/>
+      <c r="G150" s="3"/>
     </row>
     <row r="151">
       <c r="A151" s="3"/>
@@ -1411,6 +1750,8 @@
       <c r="C151" s="3"/>
       <c r="D151" s="3"/>
       <c r="E151" s="3"/>
+      <c r="F151" s="3"/>
+      <c r="G151" s="3"/>
     </row>
     <row r="152">
       <c r="A152" s="3"/>
@@ -1418,6 +1759,8 @@
       <c r="C152" s="3"/>
       <c r="D152" s="3"/>
       <c r="E152" s="3"/>
+      <c r="F152" s="3"/>
+      <c r="G152" s="3"/>
     </row>
     <row r="153">
       <c r="A153" s="3"/>
@@ -1425,6 +1768,8 @@
       <c r="C153" s="3"/>
       <c r="D153" s="3"/>
       <c r="E153" s="3"/>
+      <c r="F153" s="3"/>
+      <c r="G153" s="3"/>
     </row>
     <row r="154">
       <c r="A154" s="3"/>
@@ -1432,6 +1777,8 @@
       <c r="C154" s="3"/>
       <c r="D154" s="3"/>
       <c r="E154" s="3"/>
+      <c r="F154" s="3"/>
+      <c r="G154" s="3"/>
     </row>
     <row r="155">
       <c r="A155" s="3"/>
@@ -1439,6 +1786,8 @@
       <c r="C155" s="3"/>
       <c r="D155" s="3"/>
       <c r="E155" s="3"/>
+      <c r="F155" s="3"/>
+      <c r="G155" s="3"/>
     </row>
     <row r="156">
       <c r="A156" s="3"/>
@@ -1446,6 +1795,8 @@
       <c r="C156" s="3"/>
       <c r="D156" s="3"/>
       <c r="E156" s="3"/>
+      <c r="F156" s="3"/>
+      <c r="G156" s="3"/>
     </row>
     <row r="157">
       <c r="A157" s="3"/>
@@ -1453,6 +1804,8 @@
       <c r="C157" s="3"/>
       <c r="D157" s="3"/>
       <c r="E157" s="3"/>
+      <c r="F157" s="3"/>
+      <c r="G157" s="3"/>
     </row>
     <row r="158">
       <c r="A158" s="3"/>
@@ -1460,6 +1813,8 @@
       <c r="C158" s="3"/>
       <c r="D158" s="3"/>
       <c r="E158" s="3"/>
+      <c r="F158" s="3"/>
+      <c r="G158" s="3"/>
     </row>
     <row r="159">
       <c r="A159" s="3"/>
@@ -1467,6 +1822,8 @@
       <c r="C159" s="3"/>
       <c r="D159" s="3"/>
       <c r="E159" s="3"/>
+      <c r="F159" s="3"/>
+      <c r="G159" s="3"/>
     </row>
     <row r="160">
       <c r="A160" s="3"/>
@@ -1474,6 +1831,8 @@
       <c r="C160" s="3"/>
       <c r="D160" s="3"/>
       <c r="E160" s="3"/>
+      <c r="F160" s="3"/>
+      <c r="G160" s="3"/>
     </row>
     <row r="161">
       <c r="A161" s="3"/>
@@ -1481,6 +1840,8 @@
       <c r="C161" s="3"/>
       <c r="D161" s="3"/>
       <c r="E161" s="3"/>
+      <c r="F161" s="3"/>
+      <c r="G161" s="3"/>
     </row>
     <row r="162">
       <c r="A162" s="3"/>
@@ -1488,6 +1849,8 @@
       <c r="C162" s="3"/>
       <c r="D162" s="3"/>
       <c r="E162" s="3"/>
+      <c r="F162" s="3"/>
+      <c r="G162" s="3"/>
     </row>
     <row r="163">
       <c r="A163" s="3"/>
@@ -1495,6 +1858,8 @@
       <c r="C163" s="3"/>
       <c r="D163" s="3"/>
       <c r="E163" s="3"/>
+      <c r="F163" s="3"/>
+      <c r="G163" s="3"/>
     </row>
     <row r="164">
       <c r="A164" s="3"/>
@@ -1502,6 +1867,8 @@
       <c r="C164" s="3"/>
       <c r="D164" s="3"/>
       <c r="E164" s="3"/>
+      <c r="F164" s="3"/>
+      <c r="G164" s="3"/>
     </row>
     <row r="165">
       <c r="A165" s="3"/>
@@ -1509,6 +1876,8 @@
       <c r="C165" s="3"/>
       <c r="D165" s="3"/>
       <c r="E165" s="3"/>
+      <c r="F165" s="3"/>
+      <c r="G165" s="3"/>
     </row>
     <row r="166">
       <c r="A166" s="3"/>
@@ -1516,6 +1885,8 @@
       <c r="C166" s="3"/>
       <c r="D166" s="3"/>
       <c r="E166" s="3"/>
+      <c r="F166" s="3"/>
+      <c r="G166" s="3"/>
     </row>
     <row r="167">
       <c r="A167" s="3"/>
@@ -1523,6 +1894,8 @@
       <c r="C167" s="3"/>
       <c r="D167" s="3"/>
       <c r="E167" s="3"/>
+      <c r="F167" s="3"/>
+      <c r="G167" s="3"/>
     </row>
     <row r="168">
       <c r="A168" s="3"/>
@@ -1530,6 +1903,8 @@
       <c r="C168" s="3"/>
       <c r="D168" s="3"/>
       <c r="E168" s="3"/>
+      <c r="F168" s="3"/>
+      <c r="G168" s="3"/>
     </row>
     <row r="169">
       <c r="A169" s="3"/>
@@ -1537,6 +1912,8 @@
       <c r="C169" s="3"/>
       <c r="D169" s="3"/>
       <c r="E169" s="3"/>
+      <c r="F169" s="3"/>
+      <c r="G169" s="3"/>
     </row>
     <row r="170">
       <c r="A170" s="3"/>
@@ -1544,6 +1921,8 @@
       <c r="C170" s="3"/>
       <c r="D170" s="3"/>
       <c r="E170" s="3"/>
+      <c r="F170" s="3"/>
+      <c r="G170" s="3"/>
     </row>
     <row r="171">
       <c r="A171" s="3"/>
@@ -1551,6 +1930,8 @@
       <c r="C171" s="3"/>
       <c r="D171" s="3"/>
       <c r="E171" s="3"/>
+      <c r="F171" s="3"/>
+      <c r="G171" s="3"/>
     </row>
     <row r="172">
       <c r="A172" s="3"/>
@@ -1558,6 +1939,8 @@
       <c r="C172" s="3"/>
       <c r="D172" s="3"/>
       <c r="E172" s="3"/>
+      <c r="F172" s="3"/>
+      <c r="G172" s="3"/>
     </row>
     <row r="173">
       <c r="A173" s="3"/>
@@ -1565,6 +1948,8 @@
       <c r="C173" s="3"/>
       <c r="D173" s="3"/>
       <c r="E173" s="3"/>
+      <c r="F173" s="3"/>
+      <c r="G173" s="3"/>
     </row>
     <row r="174">
       <c r="A174" s="3"/>
@@ -1572,6 +1957,8 @@
       <c r="C174" s="3"/>
       <c r="D174" s="3"/>
       <c r="E174" s="3"/>
+      <c r="F174" s="3"/>
+      <c r="G174" s="3"/>
     </row>
     <row r="175">
       <c r="A175" s="3"/>
@@ -1579,6 +1966,8 @@
       <c r="C175" s="3"/>
       <c r="D175" s="3"/>
       <c r="E175" s="3"/>
+      <c r="F175" s="3"/>
+      <c r="G175" s="3"/>
     </row>
     <row r="176">
       <c r="A176" s="3"/>
@@ -1586,6 +1975,8 @@
       <c r="C176" s="3"/>
       <c r="D176" s="3"/>
       <c r="E176" s="3"/>
+      <c r="F176" s="3"/>
+      <c r="G176" s="3"/>
     </row>
     <row r="177">
       <c r="A177" s="3"/>
@@ -1593,6 +1984,8 @@
       <c r="C177" s="3"/>
       <c r="D177" s="3"/>
       <c r="E177" s="3"/>
+      <c r="F177" s="3"/>
+      <c r="G177" s="3"/>
     </row>
     <row r="178">
       <c r="A178" s="3"/>
@@ -1600,6 +1993,8 @@
       <c r="C178" s="3"/>
       <c r="D178" s="3"/>
       <c r="E178" s="3"/>
+      <c r="F178" s="3"/>
+      <c r="G178" s="3"/>
     </row>
     <row r="179">
       <c r="A179" s="3"/>
@@ -1607,6 +2002,8 @@
       <c r="C179" s="3"/>
       <c r="D179" s="3"/>
       <c r="E179" s="3"/>
+      <c r="F179" s="3"/>
+      <c r="G179" s="3"/>
     </row>
     <row r="180">
       <c r="A180" s="3"/>
@@ -1614,6 +2011,8 @@
       <c r="C180" s="3"/>
       <c r="D180" s="3"/>
       <c r="E180" s="3"/>
+      <c r="F180" s="3"/>
+      <c r="G180" s="3"/>
     </row>
     <row r="181">
       <c r="A181" s="3"/>
@@ -1621,6 +2020,8 @@
       <c r="C181" s="3"/>
       <c r="D181" s="3"/>
       <c r="E181" s="3"/>
+      <c r="F181" s="3"/>
+      <c r="G181" s="3"/>
     </row>
     <row r="182">
       <c r="A182" s="3"/>
@@ -1628,6 +2029,8 @@
       <c r="C182" s="3"/>
       <c r="D182" s="3"/>
       <c r="E182" s="3"/>
+      <c r="F182" s="3"/>
+      <c r="G182" s="3"/>
     </row>
     <row r="183">
       <c r="A183" s="3"/>
@@ -1635,6 +2038,8 @@
       <c r="C183" s="3"/>
       <c r="D183" s="3"/>
       <c r="E183" s="3"/>
+      <c r="F183" s="3"/>
+      <c r="G183" s="3"/>
     </row>
     <row r="184">
       <c r="A184" s="3"/>
@@ -1642,6 +2047,8 @@
       <c r="C184" s="3"/>
       <c r="D184" s="3"/>
       <c r="E184" s="3"/>
+      <c r="F184" s="3"/>
+      <c r="G184" s="3"/>
     </row>
     <row r="185">
       <c r="A185" s="3"/>
@@ -1649,6 +2056,8 @@
       <c r="C185" s="3"/>
       <c r="D185" s="3"/>
       <c r="E185" s="3"/>
+      <c r="F185" s="3"/>
+      <c r="G185" s="3"/>
     </row>
     <row r="186">
       <c r="A186" s="3"/>
@@ -1656,6 +2065,8 @@
       <c r="C186" s="3"/>
       <c r="D186" s="3"/>
       <c r="E186" s="3"/>
+      <c r="F186" s="3"/>
+      <c r="G186" s="3"/>
     </row>
     <row r="187">
       <c r="A187" s="3"/>
@@ -1663,6 +2074,8 @@
       <c r="C187" s="3"/>
       <c r="D187" s="3"/>
       <c r="E187" s="3"/>
+      <c r="F187" s="3"/>
+      <c r="G187" s="3"/>
     </row>
     <row r="188">
       <c r="A188" s="3"/>
@@ -1670,6 +2083,8 @@
       <c r="C188" s="3"/>
       <c r="D188" s="3"/>
       <c r="E188" s="3"/>
+      <c r="F188" s="3"/>
+      <c r="G188" s="3"/>
     </row>
     <row r="189">
       <c r="A189" s="3"/>
@@ -1677,6 +2092,8 @@
       <c r="C189" s="3"/>
       <c r="D189" s="3"/>
       <c r="E189" s="3"/>
+      <c r="F189" s="3"/>
+      <c r="G189" s="3"/>
     </row>
     <row r="190">
       <c r="A190" s="3"/>
@@ -1684,6 +2101,8 @@
       <c r="C190" s="3"/>
       <c r="D190" s="3"/>
       <c r="E190" s="3"/>
+      <c r="F190" s="3"/>
+      <c r="G190" s="3"/>
     </row>
     <row r="191">
       <c r="A191" s="3"/>
@@ -1691,6 +2110,8 @@
       <c r="C191" s="3"/>
       <c r="D191" s="3"/>
       <c r="E191" s="3"/>
+      <c r="F191" s="3"/>
+      <c r="G191" s="3"/>
     </row>
     <row r="192">
       <c r="A192" s="3"/>
@@ -1698,6 +2119,8 @@
       <c r="C192" s="3"/>
       <c r="D192" s="3"/>
       <c r="E192" s="3"/>
+      <c r="F192" s="3"/>
+      <c r="G192" s="3"/>
     </row>
     <row r="193">
       <c r="A193" s="3"/>
@@ -1705,6 +2128,8 @@
       <c r="C193" s="3"/>
       <c r="D193" s="3"/>
       <c r="E193" s="3"/>
+      <c r="F193" s="3"/>
+      <c r="G193" s="3"/>
     </row>
     <row r="194">
       <c r="A194" s="3"/>
@@ -1712,6 +2137,8 @@
       <c r="C194" s="3"/>
       <c r="D194" s="3"/>
       <c r="E194" s="3"/>
+      <c r="F194" s="3"/>
+      <c r="G194" s="3"/>
     </row>
     <row r="195">
       <c r="A195" s="3"/>
@@ -1719,6 +2146,8 @@
       <c r="C195" s="3"/>
       <c r="D195" s="3"/>
       <c r="E195" s="3"/>
+      <c r="F195" s="3"/>
+      <c r="G195" s="3"/>
     </row>
     <row r="196">
       <c r="A196" s="3"/>
@@ -1726,6 +2155,8 @@
       <c r="C196" s="3"/>
       <c r="D196" s="3"/>
       <c r="E196" s="3"/>
+      <c r="F196" s="3"/>
+      <c r="G196" s="3"/>
     </row>
     <row r="197">
       <c r="A197" s="3"/>
@@ -1733,6 +2164,8 @@
       <c r="C197" s="3"/>
       <c r="D197" s="3"/>
       <c r="E197" s="3"/>
+      <c r="F197" s="3"/>
+      <c r="G197" s="3"/>
     </row>
     <row r="198">
       <c r="A198" s="3"/>
@@ -1740,6 +2173,8 @@
       <c r="C198" s="3"/>
       <c r="D198" s="3"/>
       <c r="E198" s="3"/>
+      <c r="F198" s="3"/>
+      <c r="G198" s="3"/>
     </row>
     <row r="199">
       <c r="A199" s="3"/>
@@ -1747,6 +2182,8 @@
       <c r="C199" s="3"/>
       <c r="D199" s="3"/>
       <c r="E199" s="3"/>
+      <c r="F199" s="3"/>
+      <c r="G199" s="3"/>
     </row>
     <row r="200">
       <c r="A200" s="3"/>
@@ -1754,6 +2191,8 @@
       <c r="C200" s="3"/>
       <c r="D200" s="3"/>
       <c r="E200" s="3"/>
+      <c r="F200" s="3"/>
+      <c r="G200" s="3"/>
     </row>
     <row r="201">
       <c r="A201" s="3"/>
@@ -1761,6 +2200,8 @@
       <c r="C201" s="3"/>
       <c r="D201" s="3"/>
       <c r="E201" s="3"/>
+      <c r="F201" s="3"/>
+      <c r="G201" s="3"/>
     </row>
     <row r="202">
       <c r="A202" s="3"/>
@@ -1768,6 +2209,8 @@
       <c r="C202" s="3"/>
       <c r="D202" s="3"/>
       <c r="E202" s="3"/>
+      <c r="F202" s="3"/>
+      <c r="G202" s="3"/>
     </row>
     <row r="203">
       <c r="A203" s="3"/>
@@ -1775,6 +2218,8 @@
       <c r="C203" s="3"/>
       <c r="D203" s="3"/>
       <c r="E203" s="3"/>
+      <c r="F203" s="3"/>
+      <c r="G203" s="3"/>
     </row>
     <row r="204">
       <c r="A204" s="3"/>
@@ -1782,6 +2227,8 @@
       <c r="C204" s="3"/>
       <c r="D204" s="3"/>
       <c r="E204" s="3"/>
+      <c r="F204" s="3"/>
+      <c r="G204" s="3"/>
     </row>
     <row r="205">
       <c r="A205" s="3"/>
@@ -1789,6 +2236,8 @@
       <c r="C205" s="3"/>
       <c r="D205" s="3"/>
       <c r="E205" s="3"/>
+      <c r="F205" s="3"/>
+      <c r="G205" s="3"/>
     </row>
     <row r="206">
       <c r="A206" s="3"/>
@@ -1796,6 +2245,8 @@
       <c r="C206" s="3"/>
       <c r="D206" s="3"/>
       <c r="E206" s="3"/>
+      <c r="F206" s="3"/>
+      <c r="G206" s="3"/>
     </row>
     <row r="207">
       <c r="A207" s="3"/>
@@ -1803,6 +2254,8 @@
       <c r="C207" s="3"/>
       <c r="D207" s="3"/>
       <c r="E207" s="3"/>
+      <c r="F207" s="3"/>
+      <c r="G207" s="3"/>
     </row>
     <row r="208">
       <c r="A208" s="3"/>
@@ -1810,6 +2263,8 @@
       <c r="C208" s="3"/>
       <c r="D208" s="3"/>
       <c r="E208" s="3"/>
+      <c r="F208" s="3"/>
+      <c r="G208" s="3"/>
     </row>
     <row r="209">
       <c r="A209" s="3"/>
@@ -1817,6 +2272,8 @@
       <c r="C209" s="3"/>
       <c r="D209" s="3"/>
       <c r="E209" s="3"/>
+      <c r="F209" s="3"/>
+      <c r="G209" s="3"/>
     </row>
     <row r="210">
       <c r="A210" s="3"/>
@@ -1824,6 +2281,8 @@
       <c r="C210" s="3"/>
       <c r="D210" s="3"/>
       <c r="E210" s="3"/>
+      <c r="F210" s="3"/>
+      <c r="G210" s="3"/>
     </row>
     <row r="211">
       <c r="A211" s="3"/>
@@ -1831,6 +2290,8 @@
       <c r="C211" s="3"/>
       <c r="D211" s="3"/>
       <c r="E211" s="3"/>
+      <c r="F211" s="3"/>
+      <c r="G211" s="3"/>
     </row>
     <row r="212">
       <c r="A212" s="3"/>
@@ -1838,6 +2299,8 @@
       <c r="C212" s="3"/>
       <c r="D212" s="3"/>
       <c r="E212" s="3"/>
+      <c r="F212" s="3"/>
+      <c r="G212" s="3"/>
     </row>
     <row r="213">
       <c r="A213" s="3"/>
@@ -1845,6 +2308,8 @@
       <c r="C213" s="3"/>
       <c r="D213" s="3"/>
       <c r="E213" s="3"/>
+      <c r="F213" s="3"/>
+      <c r="G213" s="3"/>
     </row>
     <row r="214">
       <c r="A214" s="3"/>
@@ -1852,6 +2317,8 @@
       <c r="C214" s="3"/>
       <c r="D214" s="3"/>
       <c r="E214" s="3"/>
+      <c r="F214" s="3"/>
+      <c r="G214" s="3"/>
     </row>
     <row r="215">
       <c r="A215" s="3"/>
@@ -1859,6 +2326,8 @@
       <c r="C215" s="3"/>
       <c r="D215" s="3"/>
       <c r="E215" s="3"/>
+      <c r="F215" s="3"/>
+      <c r="G215" s="3"/>
     </row>
     <row r="216">
       <c r="A216" s="3"/>
@@ -1866,6 +2335,8 @@
       <c r="C216" s="3"/>
       <c r="D216" s="3"/>
       <c r="E216" s="3"/>
+      <c r="F216" s="3"/>
+      <c r="G216" s="3"/>
     </row>
     <row r="217">
       <c r="A217" s="3"/>
@@ -1873,6 +2344,8 @@
       <c r="C217" s="3"/>
       <c r="D217" s="3"/>
       <c r="E217" s="3"/>
+      <c r="F217" s="3"/>
+      <c r="G217" s="3"/>
     </row>
     <row r="218">
       <c r="A218" s="3"/>
@@ -1880,6 +2353,8 @@
       <c r="C218" s="3"/>
       <c r="D218" s="3"/>
       <c r="E218" s="3"/>
+      <c r="F218" s="3"/>
+      <c r="G218" s="3"/>
     </row>
     <row r="219">
       <c r="A219" s="3"/>
@@ -1887,6 +2362,8 @@
       <c r="C219" s="3"/>
       <c r="D219" s="3"/>
       <c r="E219" s="3"/>
+      <c r="F219" s="3"/>
+      <c r="G219" s="3"/>
     </row>
     <row r="220">
       <c r="A220" s="3"/>
@@ -1894,6 +2371,8 @@
       <c r="C220" s="3"/>
       <c r="D220" s="3"/>
       <c r="E220" s="3"/>
+      <c r="F220" s="3"/>
+      <c r="G220" s="3"/>
     </row>
     <row r="221">
       <c r="A221" s="3"/>
@@ -1901,6 +2380,8 @@
       <c r="C221" s="3"/>
       <c r="D221" s="3"/>
       <c r="E221" s="3"/>
+      <c r="F221" s="3"/>
+      <c r="G221" s="3"/>
     </row>
     <row r="222">
       <c r="A222" s="3"/>
@@ -1908,6 +2389,8 @@
       <c r="C222" s="3"/>
       <c r="D222" s="3"/>
       <c r="E222" s="3"/>
+      <c r="F222" s="3"/>
+      <c r="G222" s="3"/>
     </row>
     <row r="223">
       <c r="A223" s="3"/>
@@ -1915,6 +2398,8 @@
       <c r="C223" s="3"/>
       <c r="D223" s="3"/>
       <c r="E223" s="3"/>
+      <c r="F223" s="3"/>
+      <c r="G223" s="3"/>
     </row>
     <row r="224">
       <c r="A224" s="3"/>
@@ -1922,6 +2407,8 @@
       <c r="C224" s="3"/>
       <c r="D224" s="3"/>
       <c r="E224" s="3"/>
+      <c r="F224" s="3"/>
+      <c r="G224" s="3"/>
     </row>
     <row r="225">
       <c r="A225" s="3"/>
@@ -1929,6 +2416,8 @@
       <c r="C225" s="3"/>
       <c r="D225" s="3"/>
       <c r="E225" s="3"/>
+      <c r="F225" s="3"/>
+      <c r="G225" s="3"/>
     </row>
     <row r="226">
       <c r="A226" s="3"/>
@@ -1936,6 +2425,8 @@
       <c r="C226" s="3"/>
       <c r="D226" s="3"/>
       <c r="E226" s="3"/>
+      <c r="F226" s="3"/>
+      <c r="G226" s="3"/>
     </row>
     <row r="227">
       <c r="A227" s="3"/>
@@ -1943,6 +2434,8 @@
       <c r="C227" s="3"/>
       <c r="D227" s="3"/>
       <c r="E227" s="3"/>
+      <c r="F227" s="3"/>
+      <c r="G227" s="3"/>
     </row>
     <row r="228">
       <c r="A228" s="3"/>
@@ -1950,6 +2443,8 @@
       <c r="C228" s="3"/>
       <c r="D228" s="3"/>
       <c r="E228" s="3"/>
+      <c r="F228" s="3"/>
+      <c r="G228" s="3"/>
     </row>
     <row r="229">
       <c r="A229" s="3"/>
@@ -1957,6 +2452,8 @@
       <c r="C229" s="3"/>
       <c r="D229" s="3"/>
       <c r="E229" s="3"/>
+      <c r="F229" s="3"/>
+      <c r="G229" s="3"/>
     </row>
     <row r="230">
       <c r="A230" s="3"/>
@@ -1964,6 +2461,8 @@
       <c r="C230" s="3"/>
       <c r="D230" s="3"/>
       <c r="E230" s="3"/>
+      <c r="F230" s="3"/>
+      <c r="G230" s="3"/>
     </row>
     <row r="231">
       <c r="A231" s="3"/>
@@ -1971,6 +2470,8 @@
       <c r="C231" s="3"/>
       <c r="D231" s="3"/>
       <c r="E231" s="3"/>
+      <c r="F231" s="3"/>
+      <c r="G231" s="3"/>
     </row>
     <row r="232">
       <c r="A232" s="3"/>
@@ -1978,6 +2479,8 @@
       <c r="C232" s="3"/>
       <c r="D232" s="3"/>
       <c r="E232" s="3"/>
+      <c r="F232" s="3"/>
+      <c r="G232" s="3"/>
     </row>
     <row r="233">
       <c r="A233" s="3"/>
@@ -1985,6 +2488,8 @@
       <c r="C233" s="3"/>
       <c r="D233" s="3"/>
       <c r="E233" s="3"/>
+      <c r="F233" s="3"/>
+      <c r="G233" s="3"/>
     </row>
     <row r="234">
       <c r="A234" s="3"/>
@@ -1992,6 +2497,8 @@
       <c r="C234" s="3"/>
       <c r="D234" s="3"/>
       <c r="E234" s="3"/>
+      <c r="F234" s="3"/>
+      <c r="G234" s="3"/>
     </row>
     <row r="235">
       <c r="A235" s="3"/>
@@ -1999,6 +2506,8 @@
       <c r="C235" s="3"/>
       <c r="D235" s="3"/>
       <c r="E235" s="3"/>
+      <c r="F235" s="3"/>
+      <c r="G235" s="3"/>
     </row>
     <row r="236">
       <c r="A236" s="3"/>
@@ -2006,6 +2515,8 @@
       <c r="C236" s="3"/>
       <c r="D236" s="3"/>
       <c r="E236" s="3"/>
+      <c r="F236" s="3"/>
+      <c r="G236" s="3"/>
     </row>
     <row r="237">
       <c r="A237" s="3"/>
@@ -2013,6 +2524,8 @@
       <c r="C237" s="3"/>
       <c r="D237" s="3"/>
       <c r="E237" s="3"/>
+      <c r="F237" s="3"/>
+      <c r="G237" s="3"/>
     </row>
     <row r="238">
       <c r="A238" s="3"/>
@@ -2020,6 +2533,8 @@
       <c r="C238" s="3"/>
       <c r="D238" s="3"/>
       <c r="E238" s="3"/>
+      <c r="F238" s="3"/>
+      <c r="G238" s="3"/>
     </row>
     <row r="239">
       <c r="A239" s="3"/>
@@ -2027,6 +2542,8 @@
       <c r="C239" s="3"/>
       <c r="D239" s="3"/>
       <c r="E239" s="3"/>
+      <c r="F239" s="3"/>
+      <c r="G239" s="3"/>
     </row>
     <row r="240">
       <c r="A240" s="3"/>
@@ -2034,6 +2551,8 @@
       <c r="C240" s="3"/>
       <c r="D240" s="3"/>
       <c r="E240" s="3"/>
+      <c r="F240" s="3"/>
+      <c r="G240" s="3"/>
     </row>
     <row r="241">
       <c r="A241" s="3"/>
@@ -2041,6 +2560,8 @@
       <c r="C241" s="3"/>
       <c r="D241" s="3"/>
       <c r="E241" s="3"/>
+      <c r="F241" s="3"/>
+      <c r="G241" s="3"/>
     </row>
     <row r="242">
       <c r="A242" s="3"/>
@@ -2048,6 +2569,8 @@
       <c r="C242" s="3"/>
       <c r="D242" s="3"/>
       <c r="E242" s="3"/>
+      <c r="F242" s="3"/>
+      <c r="G242" s="3"/>
     </row>
     <row r="243">
       <c r="A243" s="3"/>
@@ -2055,6 +2578,8 @@
       <c r="C243" s="3"/>
       <c r="D243" s="3"/>
       <c r="E243" s="3"/>
+      <c r="F243" s="3"/>
+      <c r="G243" s="3"/>
     </row>
     <row r="244">
       <c r="A244" s="3"/>
@@ -2062,6 +2587,8 @@
       <c r="C244" s="3"/>
       <c r="D244" s="3"/>
       <c r="E244" s="3"/>
+      <c r="F244" s="3"/>
+      <c r="G244" s="3"/>
     </row>
     <row r="245">
       <c r="A245" s="3"/>
@@ -2069,6 +2596,8 @@
       <c r="C245" s="3"/>
       <c r="D245" s="3"/>
       <c r="E245" s="3"/>
+      <c r="F245" s="3"/>
+      <c r="G245" s="3"/>
     </row>
     <row r="246">
       <c r="A246" s="3"/>
@@ -2076,6 +2605,8 @@
       <c r="C246" s="3"/>
       <c r="D246" s="3"/>
       <c r="E246" s="3"/>
+      <c r="F246" s="3"/>
+      <c r="G246" s="3"/>
     </row>
     <row r="247">
       <c r="A247" s="3"/>
@@ -2083,6 +2614,8 @@
       <c r="C247" s="3"/>
       <c r="D247" s="3"/>
       <c r="E247" s="3"/>
+      <c r="F247" s="3"/>
+      <c r="G247" s="3"/>
     </row>
     <row r="248">
       <c r="A248" s="3"/>
@@ -2090,6 +2623,8 @@
       <c r="C248" s="3"/>
       <c r="D248" s="3"/>
       <c r="E248" s="3"/>
+      <c r="F248" s="3"/>
+      <c r="G248" s="3"/>
     </row>
     <row r="249">
       <c r="A249" s="3"/>
@@ -2097,6 +2632,8 @@
       <c r="C249" s="3"/>
       <c r="D249" s="3"/>
       <c r="E249" s="3"/>
+      <c r="F249" s="3"/>
+      <c r="G249" s="3"/>
     </row>
     <row r="250">
       <c r="A250" s="3"/>
@@ -2104,6 +2641,8 @@
       <c r="C250" s="3"/>
       <c r="D250" s="3"/>
       <c r="E250" s="3"/>
+      <c r="F250" s="3"/>
+      <c r="G250" s="3"/>
     </row>
     <row r="251">
       <c r="A251" s="3"/>
@@ -2111,6 +2650,8 @@
       <c r="C251" s="3"/>
       <c r="D251" s="3"/>
       <c r="E251" s="3"/>
+      <c r="F251" s="3"/>
+      <c r="G251" s="3"/>
     </row>
     <row r="252">
       <c r="A252" s="3"/>
@@ -2118,6 +2659,8 @@
       <c r="C252" s="3"/>
       <c r="D252" s="3"/>
       <c r="E252" s="3"/>
+      <c r="F252" s="3"/>
+      <c r="G252" s="3"/>
     </row>
     <row r="253">
       <c r="A253" s="3"/>
@@ -2125,6 +2668,8 @@
       <c r="C253" s="3"/>
       <c r="D253" s="3"/>
       <c r="E253" s="3"/>
+      <c r="F253" s="3"/>
+      <c r="G253" s="3"/>
     </row>
     <row r="254">
       <c r="A254" s="3"/>
@@ -2132,6 +2677,8 @@
       <c r="C254" s="3"/>
       <c r="D254" s="3"/>
       <c r="E254" s="3"/>
+      <c r="F254" s="3"/>
+      <c r="G254" s="3"/>
     </row>
     <row r="255">
       <c r="A255" s="3"/>
@@ -2139,6 +2686,8 @@
       <c r="C255" s="3"/>
       <c r="D255" s="3"/>
       <c r="E255" s="3"/>
+      <c r="F255" s="3"/>
+      <c r="G255" s="3"/>
     </row>
     <row r="256">
       <c r="A256" s="3"/>
@@ -2146,6 +2695,8 @@
       <c r="C256" s="3"/>
       <c r="D256" s="3"/>
       <c r="E256" s="3"/>
+      <c r="F256" s="3"/>
+      <c r="G256" s="3"/>
     </row>
     <row r="257">
       <c r="A257" s="3"/>
@@ -2153,6 +2704,8 @@
       <c r="C257" s="3"/>
       <c r="D257" s="3"/>
       <c r="E257" s="3"/>
+      <c r="F257" s="3"/>
+      <c r="G257" s="3"/>
     </row>
     <row r="258">
       <c r="A258" s="3"/>
@@ -2160,6 +2713,8 @@
       <c r="C258" s="3"/>
       <c r="D258" s="3"/>
       <c r="E258" s="3"/>
+      <c r="F258" s="3"/>
+      <c r="G258" s="3"/>
     </row>
     <row r="259">
       <c r="A259" s="3"/>
@@ -2167,6 +2722,8 @@
       <c r="C259" s="3"/>
       <c r="D259" s="3"/>
       <c r="E259" s="3"/>
+      <c r="F259" s="3"/>
+      <c r="G259" s="3"/>
     </row>
     <row r="260">
       <c r="A260" s="3"/>
@@ -2174,6 +2731,8 @@
       <c r="C260" s="3"/>
       <c r="D260" s="3"/>
       <c r="E260" s="3"/>
+      <c r="F260" s="3"/>
+      <c r="G260" s="3"/>
     </row>
     <row r="261">
       <c r="A261" s="3"/>
@@ -2181,6 +2740,8 @@
       <c r="C261" s="3"/>
       <c r="D261" s="3"/>
       <c r="E261" s="3"/>
+      <c r="F261" s="3"/>
+      <c r="G261" s="3"/>
     </row>
     <row r="262">
       <c r="A262" s="3"/>
@@ -2188,6 +2749,8 @@
       <c r="C262" s="3"/>
       <c r="D262" s="3"/>
       <c r="E262" s="3"/>
+      <c r="F262" s="3"/>
+      <c r="G262" s="3"/>
     </row>
     <row r="263">
       <c r="A263" s="3"/>
@@ -2195,6 +2758,8 @@
       <c r="C263" s="3"/>
       <c r="D263" s="3"/>
       <c r="E263" s="3"/>
+      <c r="F263" s="3"/>
+      <c r="G263" s="3"/>
     </row>
     <row r="264">
       <c r="A264" s="3"/>
@@ -2202,6 +2767,8 @@
       <c r="C264" s="3"/>
       <c r="D264" s="3"/>
       <c r="E264" s="3"/>
+      <c r="F264" s="3"/>
+      <c r="G264" s="3"/>
     </row>
     <row r="265">
       <c r="A265" s="3"/>
@@ -2209,6 +2776,8 @@
       <c r="C265" s="3"/>
       <c r="D265" s="3"/>
       <c r="E265" s="3"/>
+      <c r="F265" s="3"/>
+      <c r="G265" s="3"/>
     </row>
     <row r="266">
       <c r="A266" s="3"/>
@@ -2216,6 +2785,8 @@
       <c r="C266" s="3"/>
       <c r="D266" s="3"/>
       <c r="E266" s="3"/>
+      <c r="F266" s="3"/>
+      <c r="G266" s="3"/>
     </row>
     <row r="267">
       <c r="A267" s="3"/>
@@ -2223,6 +2794,8 @@
       <c r="C267" s="3"/>
       <c r="D267" s="3"/>
       <c r="E267" s="3"/>
+      <c r="F267" s="3"/>
+      <c r="G267" s="3"/>
     </row>
     <row r="268">
       <c r="A268" s="3"/>
@@ -2230,6 +2803,8 @@
       <c r="C268" s="3"/>
       <c r="D268" s="3"/>
       <c r="E268" s="3"/>
+      <c r="F268" s="3"/>
+      <c r="G268" s="3"/>
     </row>
     <row r="269">
       <c r="A269" s="3"/>
@@ -2237,6 +2812,8 @@
       <c r="C269" s="3"/>
       <c r="D269" s="3"/>
       <c r="E269" s="3"/>
+      <c r="F269" s="3"/>
+      <c r="G269" s="3"/>
     </row>
     <row r="270">
       <c r="A270" s="3"/>
@@ -2244,6 +2821,8 @@
       <c r="C270" s="3"/>
       <c r="D270" s="3"/>
       <c r="E270" s="3"/>
+      <c r="F270" s="3"/>
+      <c r="G270" s="3"/>
     </row>
     <row r="271">
       <c r="A271" s="3"/>
@@ -2251,6 +2830,8 @@
       <c r="C271" s="3"/>
       <c r="D271" s="3"/>
       <c r="E271" s="3"/>
+      <c r="F271" s="3"/>
+      <c r="G271" s="3"/>
     </row>
     <row r="272">
       <c r="A272" s="3"/>
@@ -2258,6 +2839,8 @@
       <c r="C272" s="3"/>
       <c r="D272" s="3"/>
       <c r="E272" s="3"/>
+      <c r="F272" s="3"/>
+      <c r="G272" s="3"/>
     </row>
     <row r="273">
       <c r="A273" s="3"/>
@@ -2265,6 +2848,8 @@
       <c r="C273" s="3"/>
       <c r="D273" s="3"/>
       <c r="E273" s="3"/>
+      <c r="F273" s="3"/>
+      <c r="G273" s="3"/>
     </row>
     <row r="274">
       <c r="A274" s="3"/>
@@ -2272,6 +2857,8 @@
       <c r="C274" s="3"/>
       <c r="D274" s="3"/>
       <c r="E274" s="3"/>
+      <c r="F274" s="3"/>
+      <c r="G274" s="3"/>
     </row>
     <row r="275">
       <c r="A275" s="3"/>
@@ -2279,6 +2866,8 @@
       <c r="C275" s="3"/>
       <c r="D275" s="3"/>
       <c r="E275" s="3"/>
+      <c r="F275" s="3"/>
+      <c r="G275" s="3"/>
     </row>
     <row r="276">
       <c r="A276" s="3"/>
@@ -2286,6 +2875,8 @@
       <c r="C276" s="3"/>
       <c r="D276" s="3"/>
       <c r="E276" s="3"/>
+      <c r="F276" s="3"/>
+      <c r="G276" s="3"/>
     </row>
     <row r="277">
       <c r="A277" s="3"/>
@@ -2293,6 +2884,8 @@
       <c r="C277" s="3"/>
       <c r="D277" s="3"/>
       <c r="E277" s="3"/>
+      <c r="F277" s="3"/>
+      <c r="G277" s="3"/>
     </row>
     <row r="278">
       <c r="A278" s="3"/>
@@ -2300,6 +2893,8 @@
       <c r="C278" s="3"/>
       <c r="D278" s="3"/>
       <c r="E278" s="3"/>
+      <c r="F278" s="3"/>
+      <c r="G278" s="3"/>
     </row>
     <row r="279">
       <c r="A279" s="3"/>
@@ -2307,6 +2902,8 @@
       <c r="C279" s="3"/>
       <c r="D279" s="3"/>
       <c r="E279" s="3"/>
+      <c r="F279" s="3"/>
+      <c r="G279" s="3"/>
     </row>
     <row r="280">
       <c r="A280" s="3"/>
@@ -2314,6 +2911,8 @@
       <c r="C280" s="3"/>
       <c r="D280" s="3"/>
       <c r="E280" s="3"/>
+      <c r="F280" s="3"/>
+      <c r="G280" s="3"/>
     </row>
     <row r="281">
       <c r="A281" s="3"/>
@@ -2321,6 +2920,8 @@
       <c r="C281" s="3"/>
       <c r="D281" s="3"/>
       <c r="E281" s="3"/>
+      <c r="F281" s="3"/>
+      <c r="G281" s="3"/>
     </row>
     <row r="282">
       <c r="A282" s="3"/>
@@ -2328,6 +2929,8 @@
       <c r="C282" s="3"/>
       <c r="D282" s="3"/>
       <c r="E282" s="3"/>
+      <c r="F282" s="3"/>
+      <c r="G282" s="3"/>
     </row>
     <row r="283">
       <c r="A283" s="3"/>
@@ -2335,6 +2938,8 @@
       <c r="C283" s="3"/>
       <c r="D283" s="3"/>
       <c r="E283" s="3"/>
+      <c r="F283" s="3"/>
+      <c r="G283" s="3"/>
     </row>
     <row r="284">
       <c r="A284" s="3"/>
@@ -2342,6 +2947,8 @@
       <c r="C284" s="3"/>
       <c r="D284" s="3"/>
       <c r="E284" s="3"/>
+      <c r="F284" s="3"/>
+      <c r="G284" s="3"/>
     </row>
     <row r="285">
       <c r="A285" s="3"/>
@@ -2349,6 +2956,8 @@
       <c r="C285" s="3"/>
       <c r="D285" s="3"/>
       <c r="E285" s="3"/>
+      <c r="F285" s="3"/>
+      <c r="G285" s="3"/>
     </row>
     <row r="286">
       <c r="A286" s="3"/>
@@ -2356,6 +2965,8 @@
       <c r="C286" s="3"/>
       <c r="D286" s="3"/>
       <c r="E286" s="3"/>
+      <c r="F286" s="3"/>
+      <c r="G286" s="3"/>
     </row>
     <row r="287">
       <c r="A287" s="3"/>
@@ -2363,6 +2974,8 @@
       <c r="C287" s="3"/>
       <c r="D287" s="3"/>
       <c r="E287" s="3"/>
+      <c r="F287" s="3"/>
+      <c r="G287" s="3"/>
     </row>
     <row r="288">
       <c r="A288" s="3"/>
@@ -2370,6 +2983,8 @@
       <c r="C288" s="3"/>
       <c r="D288" s="3"/>
       <c r="E288" s="3"/>
+      <c r="F288" s="3"/>
+      <c r="G288" s="3"/>
     </row>
     <row r="289">
       <c r="A289" s="3"/>
@@ -2377,6 +2992,8 @@
       <c r="C289" s="3"/>
       <c r="D289" s="3"/>
       <c r="E289" s="3"/>
+      <c r="F289" s="3"/>
+      <c r="G289" s="3"/>
     </row>
     <row r="290">
       <c r="A290" s="3"/>
@@ -2384,6 +3001,8 @@
       <c r="C290" s="3"/>
       <c r="D290" s="3"/>
       <c r="E290" s="3"/>
+      <c r="F290" s="3"/>
+      <c r="G290" s="3"/>
     </row>
     <row r="291">
       <c r="A291" s="3"/>
@@ -2391,6 +3010,8 @@
       <c r="C291" s="3"/>
       <c r="D291" s="3"/>
       <c r="E291" s="3"/>
+      <c r="F291" s="3"/>
+      <c r="G291" s="3"/>
     </row>
     <row r="292">
       <c r="A292" s="3"/>
@@ -2398,6 +3019,8 @@
       <c r="C292" s="3"/>
       <c r="D292" s="3"/>
       <c r="E292" s="3"/>
+      <c r="F292" s="3"/>
+      <c r="G292" s="3"/>
     </row>
     <row r="293">
       <c r="A293" s="3"/>
@@ -2405,6 +3028,8 @@
       <c r="C293" s="3"/>
       <c r="D293" s="3"/>
       <c r="E293" s="3"/>
+      <c r="F293" s="3"/>
+      <c r="G293" s="3"/>
     </row>
     <row r="294">
       <c r="A294" s="3"/>
@@ -2412,6 +3037,8 @@
       <c r="C294" s="3"/>
       <c r="D294" s="3"/>
       <c r="E294" s="3"/>
+      <c r="F294" s="3"/>
+      <c r="G294" s="3"/>
     </row>
     <row r="295">
       <c r="A295" s="3"/>
@@ -2419,6 +3046,8 @@
       <c r="C295" s="3"/>
       <c r="D295" s="3"/>
       <c r="E295" s="3"/>
+      <c r="F295" s="3"/>
+      <c r="G295" s="3"/>
     </row>
     <row r="296">
       <c r="A296" s="3"/>
@@ -2426,6 +3055,8 @@
       <c r="C296" s="3"/>
       <c r="D296" s="3"/>
       <c r="E296" s="3"/>
+      <c r="F296" s="3"/>
+      <c r="G296" s="3"/>
     </row>
     <row r="297">
       <c r="A297" s="3"/>
@@ -2433,6 +3064,8 @@
       <c r="C297" s="3"/>
       <c r="D297" s="3"/>
       <c r="E297" s="3"/>
+      <c r="F297" s="3"/>
+      <c r="G297" s="3"/>
     </row>
     <row r="298">
       <c r="A298" s="3"/>
@@ -2440,6 +3073,8 @@
       <c r="C298" s="3"/>
       <c r="D298" s="3"/>
       <c r="E298" s="3"/>
+      <c r="F298" s="3"/>
+      <c r="G298" s="3"/>
     </row>
     <row r="299">
       <c r="A299" s="3"/>
@@ -2447,6 +3082,8 @@
       <c r="C299" s="3"/>
       <c r="D299" s="3"/>
       <c r="E299" s="3"/>
+      <c r="F299" s="3"/>
+      <c r="G299" s="3"/>
     </row>
     <row r="300">
       <c r="A300" s="3"/>
@@ -2454,6 +3091,8 @@
       <c r="C300" s="3"/>
       <c r="D300" s="3"/>
       <c r="E300" s="3"/>
+      <c r="F300" s="3"/>
+      <c r="G300" s="3"/>
     </row>
     <row r="301">
       <c r="A301" s="3"/>
@@ -2461,6 +3100,8 @@
       <c r="C301" s="3"/>
       <c r="D301" s="3"/>
       <c r="E301" s="3"/>
+      <c r="F301" s="3"/>
+      <c r="G301" s="3"/>
     </row>
     <row r="302">
       <c r="A302" s="3"/>
@@ -2468,6 +3109,8 @@
       <c r="C302" s="3"/>
       <c r="D302" s="3"/>
       <c r="E302" s="3"/>
+      <c r="F302" s="3"/>
+      <c r="G302" s="3"/>
     </row>
     <row r="303">
       <c r="A303" s="3"/>
@@ -2475,6 +3118,8 @@
       <c r="C303" s="3"/>
       <c r="D303" s="3"/>
       <c r="E303" s="3"/>
+      <c r="F303" s="3"/>
+      <c r="G303" s="3"/>
     </row>
     <row r="304">
       <c r="A304" s="3"/>
@@ -2482,6 +3127,8 @@
       <c r="C304" s="3"/>
       <c r="D304" s="3"/>
       <c r="E304" s="3"/>
+      <c r="F304" s="3"/>
+      <c r="G304" s="3"/>
     </row>
     <row r="305">
       <c r="A305" s="3"/>
@@ -2489,6 +3136,8 @@
       <c r="C305" s="3"/>
       <c r="D305" s="3"/>
       <c r="E305" s="3"/>
+      <c r="F305" s="3"/>
+      <c r="G305" s="3"/>
     </row>
     <row r="306">
       <c r="A306" s="3"/>
@@ -2496,6 +3145,8 @@
       <c r="C306" s="3"/>
       <c r="D306" s="3"/>
       <c r="E306" s="3"/>
+      <c r="F306" s="3"/>
+      <c r="G306" s="3"/>
     </row>
     <row r="307">
       <c r="A307" s="3"/>
@@ -2503,6 +3154,8 @@
       <c r="C307" s="3"/>
       <c r="D307" s="3"/>
       <c r="E307" s="3"/>
+      <c r="F307" s="3"/>
+      <c r="G307" s="3"/>
     </row>
     <row r="308">
       <c r="A308" s="3"/>
@@ -2510,6 +3163,8 @@
       <c r="C308" s="3"/>
       <c r="D308" s="3"/>
       <c r="E308" s="3"/>
+      <c r="F308" s="3"/>
+      <c r="G308" s="3"/>
     </row>
     <row r="309">
       <c r="A309" s="3"/>
@@ -2517,6 +3172,8 @@
       <c r="C309" s="3"/>
       <c r="D309" s="3"/>
       <c r="E309" s="3"/>
+      <c r="F309" s="3"/>
+      <c r="G309" s="3"/>
     </row>
     <row r="310">
       <c r="A310" s="3"/>
@@ -2524,6 +3181,8 @@
       <c r="C310" s="3"/>
       <c r="D310" s="3"/>
       <c r="E310" s="3"/>
+      <c r="F310" s="3"/>
+      <c r="G310" s="3"/>
     </row>
     <row r="311">
       <c r="A311" s="3"/>
@@ -2531,6 +3190,8 @@
       <c r="C311" s="3"/>
       <c r="D311" s="3"/>
       <c r="E311" s="3"/>
+      <c r="F311" s="3"/>
+      <c r="G311" s="3"/>
     </row>
     <row r="312">
       <c r="A312" s="3"/>
@@ -2538,6 +3199,8 @@
       <c r="C312" s="3"/>
       <c r="D312" s="3"/>
       <c r="E312" s="3"/>
+      <c r="F312" s="3"/>
+      <c r="G312" s="3"/>
     </row>
     <row r="313">
       <c r="A313" s="3"/>
@@ -2545,6 +3208,8 @@
       <c r="C313" s="3"/>
       <c r="D313" s="3"/>
       <c r="E313" s="3"/>
+      <c r="F313" s="3"/>
+      <c r="G313" s="3"/>
     </row>
     <row r="314">
       <c r="A314" s="3"/>
@@ -2552,6 +3217,8 @@
       <c r="C314" s="3"/>
       <c r="D314" s="3"/>
       <c r="E314" s="3"/>
+      <c r="F314" s="3"/>
+      <c r="G314" s="3"/>
     </row>
     <row r="315">
       <c r="A315" s="3"/>
@@ -2559,6 +3226,8 @@
       <c r="C315" s="3"/>
       <c r="D315" s="3"/>
       <c r="E315" s="3"/>
+      <c r="F315" s="3"/>
+      <c r="G315" s="3"/>
     </row>
     <row r="316">
       <c r="A316" s="3"/>
@@ -2566,6 +3235,8 @@
       <c r="C316" s="3"/>
       <c r="D316" s="3"/>
       <c r="E316" s="3"/>
+      <c r="F316" s="3"/>
+      <c r="G316" s="3"/>
     </row>
     <row r="317">
       <c r="A317" s="3"/>
@@ -2573,6 +3244,8 @@
       <c r="C317" s="3"/>
       <c r="D317" s="3"/>
       <c r="E317" s="3"/>
+      <c r="F317" s="3"/>
+      <c r="G317" s="3"/>
     </row>
     <row r="318">
       <c r="A318" s="3"/>
@@ -2580,6 +3253,8 @@
       <c r="C318" s="3"/>
       <c r="D318" s="3"/>
       <c r="E318" s="3"/>
+      <c r="F318" s="3"/>
+      <c r="G318" s="3"/>
     </row>
     <row r="319">
       <c r="A319" s="3"/>
@@ -2587,6 +3262,8 @@
       <c r="C319" s="3"/>
       <c r="D319" s="3"/>
       <c r="E319" s="3"/>
+      <c r="F319" s="3"/>
+      <c r="G319" s="3"/>
     </row>
     <row r="320">
       <c r="A320" s="3"/>
@@ -2594,6 +3271,8 @@
       <c r="C320" s="3"/>
       <c r="D320" s="3"/>
       <c r="E320" s="3"/>
+      <c r="F320" s="3"/>
+      <c r="G320" s="3"/>
     </row>
     <row r="321">
       <c r="A321" s="3"/>
@@ -2601,6 +3280,8 @@
       <c r="C321" s="3"/>
       <c r="D321" s="3"/>
       <c r="E321" s="3"/>
+      <c r="F321" s="3"/>
+      <c r="G321" s="3"/>
     </row>
     <row r="322">
       <c r="A322" s="3"/>
@@ -2608,6 +3289,8 @@
       <c r="C322" s="3"/>
       <c r="D322" s="3"/>
       <c r="E322" s="3"/>
+      <c r="F322" s="3"/>
+      <c r="G322" s="3"/>
     </row>
     <row r="323">
       <c r="A323" s="3"/>
@@ -2615,6 +3298,8 @@
       <c r="C323" s="3"/>
       <c r="D323" s="3"/>
       <c r="E323" s="3"/>
+      <c r="F323" s="3"/>
+      <c r="G323" s="3"/>
     </row>
     <row r="324">
       <c r="A324" s="3"/>
@@ -2622,6 +3307,8 @@
       <c r="C324" s="3"/>
       <c r="D324" s="3"/>
       <c r="E324" s="3"/>
+      <c r="F324" s="3"/>
+      <c r="G324" s="3"/>
     </row>
     <row r="325">
       <c r="A325" s="3"/>
@@ -2629,6 +3316,8 @@
       <c r="C325" s="3"/>
       <c r="D325" s="3"/>
       <c r="E325" s="3"/>
+      <c r="F325" s="3"/>
+      <c r="G325" s="3"/>
     </row>
     <row r="326">
       <c r="A326" s="3"/>
@@ -2636,6 +3325,8 @@
       <c r="C326" s="3"/>
       <c r="D326" s="3"/>
       <c r="E326" s="3"/>
+      <c r="F326" s="3"/>
+      <c r="G326" s="3"/>
     </row>
     <row r="327">
       <c r="A327" s="3"/>
@@ -2643,6 +3334,8 @@
       <c r="C327" s="3"/>
       <c r="D327" s="3"/>
       <c r="E327" s="3"/>
+      <c r="F327" s="3"/>
+      <c r="G327" s="3"/>
     </row>
     <row r="328">
       <c r="A328" s="3"/>
@@ -2650,6 +3343,8 @@
       <c r="C328" s="3"/>
       <c r="D328" s="3"/>
       <c r="E328" s="3"/>
+      <c r="F328" s="3"/>
+      <c r="G328" s="3"/>
     </row>
     <row r="329">
       <c r="A329" s="3"/>
@@ -2657,6 +3352,8 @@
       <c r="C329" s="3"/>
       <c r="D329" s="3"/>
       <c r="E329" s="3"/>
+      <c r="F329" s="3"/>
+      <c r="G329" s="3"/>
     </row>
     <row r="330">
       <c r="A330" s="3"/>
@@ -2664,6 +3361,8 @@
       <c r="C330" s="3"/>
       <c r="D330" s="3"/>
       <c r="E330" s="3"/>
+      <c r="F330" s="3"/>
+      <c r="G330" s="3"/>
     </row>
     <row r="331">
       <c r="A331" s="3"/>
@@ -2671,6 +3370,8 @@
       <c r="C331" s="3"/>
       <c r="D331" s="3"/>
       <c r="E331" s="3"/>
+      <c r="F331" s="3"/>
+      <c r="G331" s="3"/>
     </row>
     <row r="332">
       <c r="A332" s="3"/>
@@ -2678,6 +3379,8 @@
       <c r="C332" s="3"/>
       <c r="D332" s="3"/>
       <c r="E332" s="3"/>
+      <c r="F332" s="3"/>
+      <c r="G332" s="3"/>
     </row>
     <row r="333">
       <c r="A333" s="3"/>
@@ -2685,6 +3388,8 @@
       <c r="C333" s="3"/>
       <c r="D333" s="3"/>
       <c r="E333" s="3"/>
+      <c r="F333" s="3"/>
+      <c r="G333" s="3"/>
     </row>
     <row r="334">
       <c r="A334" s="3"/>
@@ -2692,6 +3397,8 @@
       <c r="C334" s="3"/>
       <c r="D334" s="3"/>
       <c r="E334" s="3"/>
+      <c r="F334" s="3"/>
+      <c r="G334" s="3"/>
     </row>
     <row r="335">
       <c r="A335" s="3"/>
@@ -2699,6 +3406,8 @@
       <c r="C335" s="3"/>
       <c r="D335" s="3"/>
       <c r="E335" s="3"/>
+      <c r="F335" s="3"/>
+      <c r="G335" s="3"/>
     </row>
     <row r="336">
       <c r="A336" s="3"/>
@@ -2706,6 +3415,8 @@
       <c r="C336" s="3"/>
       <c r="D336" s="3"/>
       <c r="E336" s="3"/>
+      <c r="F336" s="3"/>
+      <c r="G336" s="3"/>
     </row>
     <row r="337">
       <c r="A337" s="3"/>
@@ -2713,6 +3424,8 @@
       <c r="C337" s="3"/>
       <c r="D337" s="3"/>
       <c r="E337" s="3"/>
+      <c r="F337" s="3"/>
+      <c r="G337" s="3"/>
     </row>
     <row r="338">
       <c r="A338" s="3"/>
@@ -2720,6 +3433,8 @@
       <c r="C338" s="3"/>
       <c r="D338" s="3"/>
       <c r="E338" s="3"/>
+      <c r="F338" s="3"/>
+      <c r="G338" s="3"/>
     </row>
     <row r="339">
       <c r="A339" s="3"/>
@@ -2727,6 +3442,8 @@
       <c r="C339" s="3"/>
       <c r="D339" s="3"/>
       <c r="E339" s="3"/>
+      <c r="F339" s="3"/>
+      <c r="G339" s="3"/>
     </row>
     <row r="340">
       <c r="A340" s="3"/>
@@ -2734,6 +3451,8 @@
       <c r="C340" s="3"/>
       <c r="D340" s="3"/>
       <c r="E340" s="3"/>
+      <c r="F340" s="3"/>
+      <c r="G340" s="3"/>
     </row>
     <row r="341">
       <c r="A341" s="3"/>
@@ -2741,6 +3460,8 @@
       <c r="C341" s="3"/>
       <c r="D341" s="3"/>
       <c r="E341" s="3"/>
+      <c r="F341" s="3"/>
+      <c r="G341" s="3"/>
     </row>
     <row r="342">
       <c r="A342" s="3"/>
@@ -2748,6 +3469,8 @@
       <c r="C342" s="3"/>
       <c r="D342" s="3"/>
       <c r="E342" s="3"/>
+      <c r="F342" s="3"/>
+      <c r="G342" s="3"/>
     </row>
     <row r="343">
       <c r="A343" s="3"/>
@@ -2755,6 +3478,8 @@
       <c r="C343" s="3"/>
       <c r="D343" s="3"/>
       <c r="E343" s="3"/>
+      <c r="F343" s="3"/>
+      <c r="G343" s="3"/>
     </row>
     <row r="344">
       <c r="A344" s="3"/>
@@ -2762,6 +3487,8 @@
       <c r="C344" s="3"/>
       <c r="D344" s="3"/>
       <c r="E344" s="3"/>
+      <c r="F344" s="3"/>
+      <c r="G344" s="3"/>
     </row>
     <row r="345">
       <c r="A345" s="3"/>
@@ -2769,6 +3496,8 @@
       <c r="C345" s="3"/>
       <c r="D345" s="3"/>
       <c r="E345" s="3"/>
+      <c r="F345" s="3"/>
+      <c r="G345" s="3"/>
     </row>
     <row r="346">
       <c r="A346" s="3"/>
@@ -2776,6 +3505,8 @@
       <c r="C346" s="3"/>
       <c r="D346" s="3"/>
       <c r="E346" s="3"/>
+      <c r="F346" s="3"/>
+      <c r="G346" s="3"/>
     </row>
     <row r="347">
       <c r="A347" s="3"/>
@@ -2783,6 +3514,8 @@
       <c r="C347" s="3"/>
       <c r="D347" s="3"/>
       <c r="E347" s="3"/>
+      <c r="F347" s="3"/>
+      <c r="G347" s="3"/>
     </row>
     <row r="348">
       <c r="A348" s="3"/>
@@ -2790,6 +3523,8 @@
       <c r="C348" s="3"/>
       <c r="D348" s="3"/>
       <c r="E348" s="3"/>
+      <c r="F348" s="3"/>
+      <c r="G348" s="3"/>
     </row>
     <row r="349">
       <c r="A349" s="3"/>
@@ -2797,6 +3532,8 @@
       <c r="C349" s="3"/>
       <c r="D349" s="3"/>
       <c r="E349" s="3"/>
+      <c r="F349" s="3"/>
+      <c r="G349" s="3"/>
     </row>
     <row r="350">
       <c r="A350" s="3"/>
@@ -2804,6 +3541,8 @@
       <c r="C350" s="3"/>
       <c r="D350" s="3"/>
       <c r="E350" s="3"/>
+      <c r="F350" s="3"/>
+      <c r="G350" s="3"/>
     </row>
     <row r="351">
       <c r="A351" s="3"/>
@@ -2811,6 +3550,8 @@
       <c r="C351" s="3"/>
       <c r="D351" s="3"/>
       <c r="E351" s="3"/>
+      <c r="F351" s="3"/>
+      <c r="G351" s="3"/>
     </row>
     <row r="352">
       <c r="A352" s="3"/>
@@ -2818,6 +3559,8 @@
       <c r="C352" s="3"/>
       <c r="D352" s="3"/>
       <c r="E352" s="3"/>
+      <c r="F352" s="3"/>
+      <c r="G352" s="3"/>
     </row>
     <row r="353">
       <c r="A353" s="3"/>
@@ -2825,6 +3568,8 @@
       <c r="C353" s="3"/>
       <c r="D353" s="3"/>
       <c r="E353" s="3"/>
+      <c r="F353" s="3"/>
+      <c r="G353" s="3"/>
     </row>
     <row r="354">
       <c r="A354" s="3"/>
@@ -2832,6 +3577,8 @@
       <c r="C354" s="3"/>
       <c r="D354" s="3"/>
       <c r="E354" s="3"/>
+      <c r="F354" s="3"/>
+      <c r="G354" s="3"/>
     </row>
     <row r="355">
       <c r="A355" s="3"/>
@@ -2839,6 +3586,8 @@
       <c r="C355" s="3"/>
       <c r="D355" s="3"/>
       <c r="E355" s="3"/>
+      <c r="F355" s="3"/>
+      <c r="G355" s="3"/>
     </row>
     <row r="356">
       <c r="A356" s="3"/>
@@ -2846,6 +3595,8 @@
       <c r="C356" s="3"/>
       <c r="D356" s="3"/>
       <c r="E356" s="3"/>
+      <c r="F356" s="3"/>
+      <c r="G356" s="3"/>
     </row>
     <row r="357">
       <c r="A357" s="3"/>
@@ -2853,6 +3604,8 @@
       <c r="C357" s="3"/>
       <c r="D357" s="3"/>
       <c r="E357" s="3"/>
+      <c r="F357" s="3"/>
+      <c r="G357" s="3"/>
     </row>
     <row r="358">
       <c r="A358" s="3"/>
@@ -2860,6 +3613,8 @@
       <c r="C358" s="3"/>
       <c r="D358" s="3"/>
       <c r="E358" s="3"/>
+      <c r="F358" s="3"/>
+      <c r="G358" s="3"/>
     </row>
     <row r="359">
       <c r="A359" s="3"/>
@@ -2867,6 +3622,8 @@
       <c r="C359" s="3"/>
       <c r="D359" s="3"/>
       <c r="E359" s="3"/>
+      <c r="F359" s="3"/>
+      <c r="G359" s="3"/>
     </row>
     <row r="360">
       <c r="A360" s="3"/>
@@ -2874,6 +3631,8 @@
       <c r="C360" s="3"/>
       <c r="D360" s="3"/>
       <c r="E360" s="3"/>
+      <c r="F360" s="3"/>
+      <c r="G360" s="3"/>
     </row>
     <row r="361">
       <c r="A361" s="3"/>
@@ -2881,6 +3640,8 @@
       <c r="C361" s="3"/>
       <c r="D361" s="3"/>
       <c r="E361" s="3"/>
+      <c r="F361" s="3"/>
+      <c r="G361" s="3"/>
     </row>
     <row r="362">
       <c r="A362" s="3"/>
@@ -2888,6 +3649,8 @@
       <c r="C362" s="3"/>
       <c r="D362" s="3"/>
       <c r="E362" s="3"/>
+      <c r="F362" s="3"/>
+      <c r="G362" s="3"/>
     </row>
     <row r="363">
       <c r="A363" s="3"/>
@@ -2895,6 +3658,8 @@
       <c r="C363" s="3"/>
       <c r="D363" s="3"/>
       <c r="E363" s="3"/>
+      <c r="F363" s="3"/>
+      <c r="G363" s="3"/>
     </row>
     <row r="364">
       <c r="A364" s="3"/>
@@ -2902,6 +3667,8 @@
       <c r="C364" s="3"/>
       <c r="D364" s="3"/>
       <c r="E364" s="3"/>
+      <c r="F364" s="3"/>
+      <c r="G364" s="3"/>
     </row>
     <row r="365">
       <c r="A365" s="3"/>
@@ -2909,6 +3676,8 @@
       <c r="C365" s="3"/>
       <c r="D365" s="3"/>
       <c r="E365" s="3"/>
+      <c r="F365" s="3"/>
+      <c r="G365" s="3"/>
     </row>
     <row r="366">
       <c r="A366" s="3"/>
@@ -2916,6 +3685,8 @@
       <c r="C366" s="3"/>
       <c r="D366" s="3"/>
       <c r="E366" s="3"/>
+      <c r="F366" s="3"/>
+      <c r="G366" s="3"/>
     </row>
     <row r="367">
       <c r="A367" s="3"/>
@@ -2923,6 +3694,8 @@
       <c r="C367" s="3"/>
       <c r="D367" s="3"/>
       <c r="E367" s="3"/>
+      <c r="F367" s="3"/>
+      <c r="G367" s="3"/>
     </row>
     <row r="368">
       <c r="A368" s="3"/>
@@ -2930,6 +3703,8 @@
       <c r="C368" s="3"/>
       <c r="D368" s="3"/>
       <c r="E368" s="3"/>
+      <c r="F368" s="3"/>
+      <c r="G368" s="3"/>
     </row>
     <row r="369">
       <c r="A369" s="3"/>
@@ -2937,6 +3712,8 @@
       <c r="C369" s="3"/>
       <c r="D369" s="3"/>
       <c r="E369" s="3"/>
+      <c r="F369" s="3"/>
+      <c r="G369" s="3"/>
     </row>
     <row r="370">
       <c r="A370" s="3"/>
@@ -2944,6 +3721,8 @@
       <c r="C370" s="3"/>
       <c r="D370" s="3"/>
       <c r="E370" s="3"/>
+      <c r="F370" s="3"/>
+      <c r="G370" s="3"/>
     </row>
     <row r="371">
       <c r="A371" s="3"/>
@@ -2951,6 +3730,8 @@
       <c r="C371" s="3"/>
       <c r="D371" s="3"/>
       <c r="E371" s="3"/>
+      <c r="F371" s="3"/>
+      <c r="G371" s="3"/>
     </row>
     <row r="372">
       <c r="A372" s="3"/>
@@ -2958,6 +3739,8 @@
       <c r="C372" s="3"/>
       <c r="D372" s="3"/>
       <c r="E372" s="3"/>
+      <c r="F372" s="3"/>
+      <c r="G372" s="3"/>
     </row>
     <row r="373">
       <c r="A373" s="3"/>
@@ -2965,6 +3748,8 @@
       <c r="C373" s="3"/>
       <c r="D373" s="3"/>
       <c r="E373" s="3"/>
+      <c r="F373" s="3"/>
+      <c r="G373" s="3"/>
     </row>
     <row r="374">
       <c r="A374" s="3"/>
@@ -2972,6 +3757,8 @@
       <c r="C374" s="3"/>
       <c r="D374" s="3"/>
       <c r="E374" s="3"/>
+      <c r="F374" s="3"/>
+      <c r="G374" s="3"/>
     </row>
     <row r="375">
       <c r="A375" s="3"/>
@@ -2979,6 +3766,8 @@
       <c r="C375" s="3"/>
       <c r="D375" s="3"/>
       <c r="E375" s="3"/>
+      <c r="F375" s="3"/>
+      <c r="G375" s="3"/>
     </row>
     <row r="376">
       <c r="A376" s="3"/>
@@ -2986,6 +3775,8 @@
       <c r="C376" s="3"/>
       <c r="D376" s="3"/>
       <c r="E376" s="3"/>
+      <c r="F376" s="3"/>
+      <c r="G376" s="3"/>
     </row>
     <row r="377">
       <c r="A377" s="3"/>
@@ -2993,6 +3784,8 @@
       <c r="C377" s="3"/>
       <c r="D377" s="3"/>
       <c r="E377" s="3"/>
+      <c r="F377" s="3"/>
+      <c r="G377" s="3"/>
     </row>
     <row r="378">
       <c r="A378" s="3"/>
@@ -3000,6 +3793,8 @@
       <c r="C378" s="3"/>
       <c r="D378" s="3"/>
       <c r="E378" s="3"/>
+      <c r="F378" s="3"/>
+      <c r="G378" s="3"/>
     </row>
     <row r="379">
       <c r="A379" s="4"/>
@@ -3007,6 +3802,8 @@
       <c r="C379" s="3"/>
       <c r="D379" s="3"/>
       <c r="E379" s="3"/>
+      <c r="F379" s="3"/>
+      <c r="G379" s="3"/>
     </row>
     <row r="380">
       <c r="A380" s="3"/>
@@ -3014,6 +3811,8 @@
       <c r="C380" s="3"/>
       <c r="D380" s="3"/>
       <c r="E380" s="3"/>
+      <c r="F380" s="3"/>
+      <c r="G380" s="3"/>
     </row>
     <row r="381">
       <c r="A381" s="3"/>
@@ -3021,6 +3820,8 @@
       <c r="C381" s="3"/>
       <c r="D381" s="3"/>
       <c r="E381" s="3"/>
+      <c r="F381" s="3"/>
+      <c r="G381" s="3"/>
     </row>
     <row r="382">
       <c r="A382" s="3"/>
@@ -3028,6 +3829,8 @@
       <c r="C382" s="3"/>
       <c r="D382" s="3"/>
       <c r="E382" s="3"/>
+      <c r="F382" s="3"/>
+      <c r="G382" s="3"/>
     </row>
     <row r="383">
       <c r="A383" s="3"/>
@@ -3035,6 +3838,8 @@
       <c r="C383" s="3"/>
       <c r="D383" s="3"/>
       <c r="E383" s="3"/>
+      <c r="F383" s="3"/>
+      <c r="G383" s="3"/>
     </row>
     <row r="384">
       <c r="A384" s="3"/>
@@ -3042,6 +3847,8 @@
       <c r="C384" s="3"/>
       <c r="D384" s="3"/>
       <c r="E384" s="3"/>
+      <c r="F384" s="3"/>
+      <c r="G384" s="3"/>
     </row>
     <row r="385">
       <c r="A385" s="3"/>
@@ -3049,6 +3856,8 @@
       <c r="C385" s="3"/>
       <c r="D385" s="3"/>
       <c r="E385" s="3"/>
+      <c r="F385" s="3"/>
+      <c r="G385" s="3"/>
     </row>
     <row r="386">
       <c r="A386" s="3"/>
@@ -3056,6 +3865,8 @@
       <c r="C386" s="3"/>
       <c r="D386" s="3"/>
       <c r="E386" s="3"/>
+      <c r="F386" s="3"/>
+      <c r="G386" s="3"/>
     </row>
     <row r="387">
       <c r="A387" s="3"/>
@@ -3063,6 +3874,8 @@
       <c r="C387" s="3"/>
       <c r="D387" s="3"/>
       <c r="E387" s="3"/>
+      <c r="F387" s="3"/>
+      <c r="G387" s="3"/>
     </row>
     <row r="388">
       <c r="A388" s="3"/>
@@ -3070,6 +3883,8 @@
       <c r="C388" s="3"/>
       <c r="D388" s="3"/>
       <c r="E388" s="3"/>
+      <c r="F388" s="3"/>
+      <c r="G388" s="3"/>
     </row>
     <row r="389">
       <c r="A389" s="3"/>
@@ -3077,6 +3892,8 @@
       <c r="C389" s="3"/>
       <c r="D389" s="3"/>
       <c r="E389" s="3"/>
+      <c r="F389" s="3"/>
+      <c r="G389" s="3"/>
     </row>
     <row r="390">
       <c r="A390" s="3"/>
@@ -3084,6 +3901,8 @@
       <c r="C390" s="3"/>
       <c r="D390" s="3"/>
       <c r="E390" s="3"/>
+      <c r="F390" s="3"/>
+      <c r="G390" s="3"/>
     </row>
     <row r="391">
       <c r="A391" s="3"/>
@@ -3091,6 +3910,8 @@
       <c r="C391" s="3"/>
       <c r="D391" s="3"/>
       <c r="E391" s="3"/>
+      <c r="F391" s="3"/>
+      <c r="G391" s="3"/>
     </row>
     <row r="392">
       <c r="A392" s="3"/>
@@ -3098,6 +3919,8 @@
       <c r="C392" s="3"/>
       <c r="D392" s="3"/>
       <c r="E392" s="3"/>
+      <c r="F392" s="3"/>
+      <c r="G392" s="3"/>
     </row>
     <row r="393">
       <c r="A393" s="3"/>
@@ -3105,6 +3928,8 @@
       <c r="C393" s="3"/>
       <c r="D393" s="3"/>
       <c r="E393" s="3"/>
+      <c r="F393" s="3"/>
+      <c r="G393" s="3"/>
     </row>
     <row r="394">
       <c r="A394" s="3"/>
@@ -3112,6 +3937,8 @@
       <c r="C394" s="3"/>
       <c r="D394" s="3"/>
       <c r="E394" s="3"/>
+      <c r="F394" s="3"/>
+      <c r="G394" s="3"/>
     </row>
     <row r="395">
       <c r="A395" s="3"/>
@@ -3119,6 +3946,8 @@
       <c r="C395" s="3"/>
       <c r="D395" s="3"/>
       <c r="E395" s="3"/>
+      <c r="F395" s="3"/>
+      <c r="G395" s="3"/>
     </row>
     <row r="396">
       <c r="A396" s="3"/>
@@ -3126,6 +3955,8 @@
       <c r="C396" s="3"/>
       <c r="D396" s="3"/>
       <c r="E396" s="3"/>
+      <c r="F396" s="3"/>
+      <c r="G396" s="3"/>
     </row>
     <row r="397">
       <c r="A397" s="3"/>
@@ -3133,6 +3964,8 @@
       <c r="C397" s="3"/>
       <c r="D397" s="3"/>
       <c r="E397" s="3"/>
+      <c r="F397" s="3"/>
+      <c r="G397" s="3"/>
     </row>
     <row r="398">
       <c r="A398" s="3"/>
@@ -3140,6 +3973,8 @@
       <c r="C398" s="3"/>
       <c r="D398" s="3"/>
       <c r="E398" s="3"/>
+      <c r="F398" s="3"/>
+      <c r="G398" s="3"/>
     </row>
     <row r="399">
       <c r="A399" s="3"/>
@@ -3147,6 +3982,8 @@
       <c r="C399" s="3"/>
       <c r="D399" s="3"/>
       <c r="E399" s="3"/>
+      <c r="F399" s="3"/>
+      <c r="G399" s="3"/>
     </row>
     <row r="400">
       <c r="A400" s="3"/>
@@ -3154,17 +3991,27 @@
       <c r="C400" s="3"/>
       <c r="D400" s="3"/>
       <c r="E400" s="3"/>
+      <c r="F400" s="3"/>
+      <c r="G400" s="3"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(B2))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2:B400">
+      <formula1>"Pendapatan,Pengeluaran"</formula1>
+    </dataValidation>
     <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Masukkan angka tanpa titik/koma (contoh: 1000000)" sqref="C2:C400">
       <formula1>0.0</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt=" “Tanggal tidak boleh melebihi hari ini.”" sqref="A2:A400">
       <formula1>A2&lt;=TODAY()</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2:B400">
-      <formula1>"Pemasukan,Pengeluaran"</formula1>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E400">
+      <formula1>"Iuran,Lainnya"</formula1>
     </dataValidation>
   </dataValidations>
   <drawing r:id="rId2"/>

</xml_diff>